<commit_message>
Hecha la escena de sala secreta 1 y programada en un script. Hecha la estructura basica del programa.
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\MAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1011,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1223,6 +1223,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1232,6 +1250,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,9 +1307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1271,51 +1316,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,7 +1338,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1382,40 +1384,40 @@
                   <c:v>36.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.049999999999997</c:v>
+                  <c:v>35.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.979999999999997</c:v>
+                  <c:v>35.879999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.979999999999997</c:v>
+                  <c:v>35.879999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.479999999999997</c:v>
+                  <c:v>33.379999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.835000000000001</c:v>
+                  <c:v>25.904999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1476,6 +1478,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1532,7 +1535,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1607,23 +1610,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1659,23 +1645,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1854,11 +1823,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U107" sqref="U107"/>
+    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q127" sqref="Q127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
@@ -1884,22 +1853,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="85" t="s">
+      <c r="J2" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="87"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="93"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -1970,7 +1939,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="110" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="67" t="s">
@@ -2021,8 +1990,8 @@
       <c r="W4" s="73"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="95"/>
-      <c r="C5" s="97" t="s">
+      <c r="B5" s="111"/>
+      <c r="C5" s="94" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="56" t="s">
@@ -2072,8 +2041,8 @@
       <c r="W5" s="30"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="95"/>
-      <c r="C6" s="98"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="113"/>
       <c r="D6" s="17" t="s">
         <v>22</v>
       </c>
@@ -2121,7 +2090,7 @@
       <c r="W6" s="30"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="95"/>
+      <c r="B7" s="111"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2170,7 +2139,7 @@
       <c r="W7" s="30"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="95"/>
+      <c r="B8" s="111"/>
       <c r="C8" s="57" t="s">
         <v>18</v>
       </c>
@@ -2219,7 +2188,7 @@
       <c r="W8" s="30"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="95"/>
+      <c r="B9" s="111"/>
       <c r="C9" s="57" t="s">
         <v>17</v>
       </c>
@@ -2268,7 +2237,7 @@
       <c r="W9" s="30"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="95"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="57" t="s">
         <v>16</v>
       </c>
@@ -2317,7 +2286,7 @@
       <c r="W10" s="30"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="96"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="39" t="s">
         <v>111</v>
       </c>
@@ -2366,7 +2335,7 @@
       <c r="W11" s="49"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="107" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="74" t="s">
@@ -2417,7 +2386,7 @@
       <c r="W12" s="76"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="92"/>
+      <c r="B13" s="108"/>
       <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
@@ -2466,8 +2435,8 @@
       <c r="W13" s="31"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B14" s="92"/>
-      <c r="C14" s="97" t="s">
+      <c r="B14" s="108"/>
+      <c r="C14" s="94" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="55" t="s">
@@ -2517,8 +2486,8 @@
       <c r="W14" s="33"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="93"/>
-      <c r="C15" s="101"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="40" t="s">
         <v>119</v>
       </c>
@@ -2566,7 +2535,7 @@
       <c r="W15" s="45"/>
     </row>
     <row r="16" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="104" t="s">
         <v>121</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -2633,7 +2602,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="88"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
@@ -2698,7 +2667,7 @@
       </c>
     </row>
     <row r="18" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="88"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2763,7 +2732,7 @@
       </c>
     </row>
     <row r="19" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="88"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
@@ -2828,7 +2797,7 @@
       </c>
     </row>
     <row r="20" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="88"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -2893,7 +2862,7 @@
       </c>
     </row>
     <row r="21" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="88"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
@@ -2958,7 +2927,7 @@
       </c>
     </row>
     <row r="22" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="88"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
@@ -3023,7 +2992,7 @@
       </c>
     </row>
     <row r="23" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="88"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -3088,7 +3057,7 @@
       </c>
     </row>
     <row r="24" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="88"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
@@ -3153,7 +3122,7 @@
       </c>
     </row>
     <row r="25" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="88"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3218,7 +3187,7 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="88"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3283,7 +3252,7 @@
       </c>
     </row>
     <row r="27" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="88"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
@@ -3348,7 +3317,7 @@
       </c>
     </row>
     <row r="28" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="88"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
@@ -3413,7 +3382,7 @@
       </c>
     </row>
     <row r="29" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="88"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
@@ -3478,7 +3447,7 @@
       </c>
     </row>
     <row r="30" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="88"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
@@ -3543,7 +3512,7 @@
       </c>
     </row>
     <row r="31" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="88"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
@@ -3608,7 +3577,7 @@
       </c>
     </row>
     <row r="32" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="88"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3673,7 +3642,7 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="88"/>
+      <c r="B33" s="104"/>
       <c r="C33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3738,7 +3707,7 @@
       </c>
     </row>
     <row r="34" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="88"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3803,7 +3772,7 @@
       </c>
     </row>
     <row r="35" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="88"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
@@ -3868,7 +3837,7 @@
       </c>
     </row>
     <row r="36" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="88"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="4" t="s">
         <v>48</v>
       </c>
@@ -3933,7 +3902,7 @@
       </c>
     </row>
     <row r="37" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="88"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
@@ -3998,7 +3967,7 @@
       </c>
     </row>
     <row r="38" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="88"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4063,7 +4032,7 @@
       </c>
     </row>
     <row r="39" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="88"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="4" t="s">
         <v>51</v>
       </c>
@@ -4128,7 +4097,7 @@
       </c>
     </row>
     <row r="40" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="88"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="4" t="s">
         <v>52</v>
       </c>
@@ -4193,7 +4162,7 @@
       </c>
     </row>
     <row r="41" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="88"/>
+      <c r="B41" s="104"/>
       <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4258,7 +4227,7 @@
       </c>
     </row>
     <row r="42" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="88"/>
+      <c r="B42" s="104"/>
       <c r="C42" s="4" t="s">
         <v>54</v>
       </c>
@@ -4323,7 +4292,7 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="88"/>
+      <c r="B43" s="104"/>
       <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
@@ -4388,7 +4357,7 @@
       </c>
     </row>
     <row r="44" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="88"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="4" t="s">
         <v>56</v>
       </c>
@@ -4453,7 +4422,7 @@
       </c>
     </row>
     <row r="45" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="88"/>
+      <c r="B45" s="104"/>
       <c r="C45" s="4" t="s">
         <v>57</v>
       </c>
@@ -4518,7 +4487,7 @@
       </c>
     </row>
     <row r="46" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="88"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
@@ -4583,7 +4552,7 @@
       </c>
     </row>
     <row r="47" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="88"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="4" t="s">
         <v>59</v>
       </c>
@@ -4648,7 +4617,7 @@
       </c>
     </row>
     <row r="48" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="88"/>
+      <c r="B48" s="104"/>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
@@ -4713,7 +4682,7 @@
       </c>
     </row>
     <row r="49" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="88"/>
+      <c r="B49" s="104"/>
       <c r="C49" s="4" t="s">
         <v>61</v>
       </c>
@@ -4778,7 +4747,7 @@
       </c>
     </row>
     <row r="50" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="88"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="4" t="s">
         <v>62</v>
       </c>
@@ -4843,7 +4812,7 @@
       </c>
     </row>
     <row r="51" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="88"/>
+      <c r="B51" s="104"/>
       <c r="C51" s="18" t="s">
         <v>63</v>
       </c>
@@ -4892,7 +4861,7 @@
       <c r="W51" s="31"/>
     </row>
     <row r="52" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="88"/>
+      <c r="B52" s="104"/>
       <c r="C52" s="18" t="s">
         <v>79</v>
       </c>
@@ -4941,7 +4910,7 @@
       <c r="W52" s="31"/>
     </row>
     <row r="53" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="88"/>
+      <c r="B53" s="104"/>
       <c r="C53" s="18" t="s">
         <v>80</v>
       </c>
@@ -4990,7 +4959,7 @@
       <c r="W53" s="31"/>
     </row>
     <row r="54" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="88"/>
+      <c r="B54" s="104"/>
       <c r="C54" s="18" t="s">
         <v>81</v>
       </c>
@@ -5039,7 +5008,7 @@
       <c r="W54" s="31"/>
     </row>
     <row r="55" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="88"/>
+      <c r="B55" s="104"/>
       <c r="C55" s="18" t="s">
         <v>82</v>
       </c>
@@ -5088,7 +5057,7 @@
       <c r="W55" s="31"/>
     </row>
     <row r="56" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="88"/>
+      <c r="B56" s="104"/>
       <c r="C56" s="18" t="s">
         <v>83</v>
       </c>
@@ -5137,7 +5106,7 @@
       <c r="W56" s="31"/>
     </row>
     <row r="57" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="88"/>
+      <c r="B57" s="104"/>
       <c r="C57" s="18" t="s">
         <v>84</v>
       </c>
@@ -5186,7 +5155,7 @@
       <c r="W57" s="31"/>
     </row>
     <row r="58" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="88"/>
+      <c r="B58" s="104"/>
       <c r="C58" s="18" t="s">
         <v>85</v>
       </c>
@@ -5235,7 +5204,7 @@
       <c r="W58" s="31"/>
     </row>
     <row r="59" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="88"/>
+      <c r="B59" s="104"/>
       <c r="C59" s="18" t="s">
         <v>86</v>
       </c>
@@ -5284,7 +5253,7 @@
       <c r="W59" s="31"/>
     </row>
     <row r="60" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="88"/>
+      <c r="B60" s="104"/>
       <c r="C60" s="18" t="s">
         <v>87</v>
       </c>
@@ -5333,7 +5302,7 @@
       <c r="W60" s="31"/>
     </row>
     <row r="61" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="88"/>
+      <c r="B61" s="104"/>
       <c r="C61" s="18" t="s">
         <v>88</v>
       </c>
@@ -5382,7 +5351,7 @@
       <c r="W61" s="31"/>
     </row>
     <row r="62" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="88"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="18" t="s">
         <v>89</v>
       </c>
@@ -5431,7 +5400,7 @@
       <c r="W62" s="31"/>
     </row>
     <row r="63" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="88"/>
+      <c r="B63" s="104"/>
       <c r="C63" s="18" t="s">
         <v>90</v>
       </c>
@@ -5480,7 +5449,7 @@
       <c r="W63" s="31"/>
     </row>
     <row r="64" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="88"/>
+      <c r="B64" s="104"/>
       <c r="C64" s="18" t="s">
         <v>91</v>
       </c>
@@ -5529,7 +5498,7 @@
       <c r="W64" s="31"/>
     </row>
     <row r="65" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="89"/>
+      <c r="B65" s="105"/>
       <c r="C65" s="39" t="s">
         <v>92</v>
       </c>
@@ -5578,7 +5547,7 @@
       <c r="W65" s="45"/>
     </row>
     <row r="66" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="90" t="s">
+      <c r="B66" s="106" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="35" t="s">
@@ -5599,7 +5568,7 @@
       </c>
       <c r="I66" s="36">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.83</v>
       </c>
       <c r="J66" s="60">
         <v>0</v>
@@ -5619,17 +5588,19 @@
       <c r="O66" s="60">
         <v>0</v>
       </c>
-      <c r="P66" s="37"/>
-      <c r="Q66" s="37"/>
-      <c r="R66" s="37"/>
-      <c r="S66" s="37"/>
-      <c r="T66" s="37"/>
-      <c r="U66" s="37"/>
-      <c r="V66" s="37"/>
-      <c r="W66" s="38"/>
+      <c r="P66" s="83">
+        <v>1.83</v>
+      </c>
+      <c r="Q66" s="83"/>
+      <c r="R66" s="83"/>
+      <c r="S66" s="83"/>
+      <c r="T66" s="83"/>
+      <c r="U66" s="83"/>
+      <c r="V66" s="83"/>
+      <c r="W66" s="116"/>
     </row>
     <row r="67" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="88"/>
+      <c r="B67" s="104"/>
       <c r="C67" s="18" t="s">
         <v>66</v>
       </c>
@@ -5678,7 +5649,7 @@
       <c r="W67" s="31"/>
     </row>
     <row r="68" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="88"/>
+      <c r="B68" s="104"/>
       <c r="C68" s="18" t="s">
         <v>67</v>
       </c>
@@ -5727,7 +5698,7 @@
       <c r="W68" s="31"/>
     </row>
     <row r="69" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="88"/>
+      <c r="B69" s="104"/>
       <c r="C69" s="18" t="s">
         <v>68</v>
       </c>
@@ -5776,7 +5747,7 @@
       <c r="W69" s="31"/>
     </row>
     <row r="70" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="88"/>
+      <c r="B70" s="104"/>
       <c r="C70" s="18" t="s">
         <v>69</v>
       </c>
@@ -5825,7 +5796,7 @@
       <c r="W70" s="31"/>
     </row>
     <row r="71" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="88"/>
+      <c r="B71" s="104"/>
       <c r="C71" s="18" t="s">
         <v>70</v>
       </c>
@@ -5874,7 +5845,7 @@
       <c r="W71" s="31"/>
     </row>
     <row r="72" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="88"/>
+      <c r="B72" s="104"/>
       <c r="C72" s="18" t="s">
         <v>71</v>
       </c>
@@ -5923,7 +5894,7 @@
       <c r="W72" s="31"/>
     </row>
     <row r="73" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="88"/>
+      <c r="B73" s="104"/>
       <c r="C73" s="18" t="s">
         <v>72</v>
       </c>
@@ -5972,7 +5943,7 @@
       <c r="W73" s="31"/>
     </row>
     <row r="74" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="88"/>
+      <c r="B74" s="104"/>
       <c r="C74" s="18" t="s">
         <v>73</v>
       </c>
@@ -6021,7 +5992,7 @@
       <c r="W74" s="31"/>
     </row>
     <row r="75" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="88"/>
+      <c r="B75" s="104"/>
       <c r="C75" s="18" t="s">
         <v>74</v>
       </c>
@@ -6070,7 +6041,7 @@
       <c r="W75" s="31"/>
     </row>
     <row r="76" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="88"/>
+      <c r="B76" s="104"/>
       <c r="C76" s="18" t="s">
         <v>75</v>
       </c>
@@ -6119,7 +6090,7 @@
       <c r="W76" s="31"/>
     </row>
     <row r="77" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="88"/>
+      <c r="B77" s="104"/>
       <c r="C77" s="18" t="s">
         <v>76</v>
       </c>
@@ -6168,7 +6139,7 @@
       <c r="W77" s="31"/>
     </row>
     <row r="78" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="88"/>
+      <c r="B78" s="104"/>
       <c r="C78" s="18" t="s">
         <v>77</v>
       </c>
@@ -6217,7 +6188,7 @@
       <c r="W78" s="31"/>
     </row>
     <row r="79" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="89"/>
+      <c r="B79" s="105"/>
       <c r="C79" s="39" t="s">
         <v>78</v>
       </c>
@@ -6266,7 +6237,7 @@
       <c r="W79" s="45"/>
     </row>
     <row r="80" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="102" t="s">
+      <c r="B80" s="96" t="s">
         <v>93</v>
       </c>
       <c r="C80" s="6" t="s">
@@ -6307,33 +6278,33 @@
       <c r="O80" s="60">
         <v>0</v>
       </c>
-      <c r="P80" s="112">
+      <c r="P80" s="87">
         <v>0.05</v>
       </c>
-      <c r="Q80" s="112">
-        <v>0</v>
-      </c>
-      <c r="R80" s="112">
-        <v>0</v>
-      </c>
-      <c r="S80" s="112">
-        <v>0</v>
-      </c>
-      <c r="T80" s="112">
-        <v>0</v>
-      </c>
-      <c r="U80" s="112">
-        <v>0</v>
-      </c>
-      <c r="V80" s="112">
-        <v>0</v>
-      </c>
-      <c r="W80" s="112">
+      <c r="Q80" s="87">
+        <v>0</v>
+      </c>
+      <c r="R80" s="87">
+        <v>0</v>
+      </c>
+      <c r="S80" s="87">
+        <v>0</v>
+      </c>
+      <c r="T80" s="87">
+        <v>0</v>
+      </c>
+      <c r="U80" s="87">
+        <v>0</v>
+      </c>
+      <c r="V80" s="87">
+        <v>0</v>
+      </c>
+      <c r="W80" s="87">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="103"/>
+      <c r="B81" s="97"/>
       <c r="C81" s="4" t="s">
         <v>28</v>
       </c>
@@ -6398,7 +6369,7 @@
       </c>
     </row>
     <row r="82" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="103"/>
+      <c r="B82" s="97"/>
       <c r="C82" s="4" t="s">
         <v>30</v>
       </c>
@@ -6463,7 +6434,7 @@
       </c>
     </row>
     <row r="83" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="103"/>
+      <c r="B83" s="97"/>
       <c r="C83" s="4" t="s">
         <v>31</v>
       </c>
@@ -6528,7 +6499,7 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="103"/>
+      <c r="B84" s="97"/>
       <c r="C84" s="4" t="s">
         <v>32</v>
       </c>
@@ -6593,7 +6564,7 @@
       </c>
     </row>
     <row r="85" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="103"/>
+      <c r="B85" s="97"/>
       <c r="C85" s="4" t="s">
         <v>33</v>
       </c>
@@ -6658,7 +6629,7 @@
       </c>
     </row>
     <row r="86" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="103"/>
+      <c r="B86" s="97"/>
       <c r="C86" s="4" t="s">
         <v>34</v>
       </c>
@@ -6723,7 +6694,7 @@
       </c>
     </row>
     <row r="87" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="103"/>
+      <c r="B87" s="97"/>
       <c r="C87" s="4" t="s">
         <v>35</v>
       </c>
@@ -6788,7 +6759,7 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="103"/>
+      <c r="B88" s="97"/>
       <c r="C88" s="4" t="s">
         <v>36</v>
       </c>
@@ -6853,7 +6824,7 @@
       </c>
     </row>
     <row r="89" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="103"/>
+      <c r="B89" s="97"/>
       <c r="C89" s="4" t="s">
         <v>37</v>
       </c>
@@ -6918,7 +6889,7 @@
       </c>
     </row>
     <row r="90" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="103"/>
+      <c r="B90" s="97"/>
       <c r="C90" s="4" t="s">
         <v>38</v>
       </c>
@@ -6983,7 +6954,7 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="103"/>
+      <c r="B91" s="97"/>
       <c r="C91" s="4" t="s">
         <v>39</v>
       </c>
@@ -7048,7 +7019,7 @@
       </c>
     </row>
     <row r="92" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="103"/>
+      <c r="B92" s="97"/>
       <c r="C92" s="4" t="s">
         <v>40</v>
       </c>
@@ -7108,12 +7079,12 @@
       <c r="V92" s="84">
         <v>0</v>
       </c>
-      <c r="W92" s="111">
+      <c r="W92" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="103"/>
+      <c r="B93" s="97"/>
       <c r="C93" s="4" t="s">
         <v>41</v>
       </c>
@@ -7173,12 +7144,12 @@
       <c r="V93" s="84">
         <v>0</v>
       </c>
-      <c r="W93" s="111">
+      <c r="W93" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="103"/>
+      <c r="B94" s="97"/>
       <c r="C94" s="4" t="s">
         <v>42</v>
       </c>
@@ -7217,7 +7188,7 @@
       <c r="O94" s="58">
         <v>0</v>
       </c>
-      <c r="P94" s="112">
+      <c r="P94" s="87">
         <v>0.03</v>
       </c>
       <c r="Q94" s="84">
@@ -7238,12 +7209,12 @@
       <c r="V94" s="84">
         <v>0</v>
       </c>
-      <c r="W94" s="111">
+      <c r="W94" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="103"/>
+      <c r="B95" s="97"/>
       <c r="C95" s="4" t="s">
         <v>43</v>
       </c>
@@ -7282,7 +7253,7 @@
       <c r="O95" s="58">
         <v>0</v>
       </c>
-      <c r="P95" s="112">
+      <c r="P95" s="87">
         <v>0.03</v>
       </c>
       <c r="Q95" s="84">
@@ -7303,12 +7274,12 @@
       <c r="V95" s="84">
         <v>0</v>
       </c>
-      <c r="W95" s="111">
+      <c r="W95" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="103"/>
+      <c r="B96" s="97"/>
       <c r="C96" s="4" t="s">
         <v>122</v>
       </c>
@@ -7344,7 +7315,7 @@
       <c r="N96" s="58">
         <v>0</v>
       </c>
-      <c r="O96" s="110">
+      <c r="O96" s="85">
         <v>2.5</v>
       </c>
       <c r="P96" s="84">
@@ -7368,12 +7339,12 @@
       <c r="V96" s="84">
         <v>0</v>
       </c>
-      <c r="W96" s="111">
+      <c r="W96" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="103"/>
+      <c r="B97" s="97"/>
       <c r="C97" s="4" t="s">
         <v>123</v>
       </c>
@@ -7433,12 +7404,12 @@
       <c r="V97" s="84">
         <v>0</v>
       </c>
-      <c r="W97" s="111">
+      <c r="W97" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="103"/>
+      <c r="B98" s="97"/>
       <c r="C98" s="4" t="s">
         <v>44</v>
       </c>
@@ -7498,12 +7469,12 @@
       <c r="V98" s="84">
         <v>0</v>
       </c>
-      <c r="W98" s="111">
+      <c r="W98" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="104"/>
+      <c r="B99" s="98"/>
       <c r="C99" s="39" t="s">
         <v>94</v>
       </c>
@@ -7552,10 +7523,10 @@
       <c r="W99" s="45"/>
     </row>
     <row r="100" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="107" t="s">
+      <c r="B100" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="C100" s="105" t="s">
+      <c r="C100" s="99" t="s">
         <v>96</v>
       </c>
       <c r="D100" s="6" t="s">
@@ -7605,8 +7576,8 @@
       <c r="W100" s="38"/>
     </row>
     <row r="101" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="107"/>
-      <c r="C101" s="106"/>
+      <c r="B101" s="101"/>
+      <c r="C101" s="100"/>
       <c r="D101" s="4" t="s">
         <v>98</v>
       </c>
@@ -7654,8 +7625,8 @@
       <c r="W101" s="31"/>
     </row>
     <row r="102" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="107"/>
-      <c r="C102" s="106"/>
+      <c r="B102" s="101"/>
+      <c r="C102" s="100"/>
       <c r="D102" s="4" t="s">
         <v>99</v>
       </c>
@@ -7703,7 +7674,7 @@
       <c r="W102" s="31"/>
     </row>
     <row r="103" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="107"/>
+      <c r="B103" s="101"/>
       <c r="C103" s="18" t="s">
         <v>117</v>
       </c>
@@ -7752,7 +7723,7 @@
       <c r="W103" s="31"/>
     </row>
     <row r="104" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="107"/>
+      <c r="B104" s="101"/>
       <c r="C104" s="18" t="s">
         <v>100</v>
       </c>
@@ -7801,7 +7772,7 @@
       <c r="W104" s="31"/>
     </row>
     <row r="105" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="107"/>
+      <c r="B105" s="101"/>
       <c r="C105" s="18" t="s">
         <v>101</v>
       </c>
@@ -7850,7 +7821,7 @@
       <c r="W105" s="31"/>
     </row>
     <row r="106" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="107"/>
+      <c r="B106" s="101"/>
       <c r="C106" s="18" t="s">
         <v>102</v>
       </c>
@@ -7899,7 +7870,7 @@
       <c r="W106" s="31"/>
     </row>
     <row r="107" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="107"/>
+      <c r="B107" s="101"/>
       <c r="C107" s="18" t="s">
         <v>103</v>
       </c>
@@ -7948,7 +7919,7 @@
       <c r="W107" s="31"/>
     </row>
     <row r="108" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="108"/>
+      <c r="B108" s="102"/>
       <c r="C108" s="18" t="s">
         <v>104</v>
       </c>
@@ -8067,7 +8038,7 @@
       </c>
       <c r="I110" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J110" s="58">
         <v>0</v>
@@ -8075,26 +8046,26 @@
       <c r="K110" s="58">
         <v>0</v>
       </c>
-      <c r="L110" s="58">
-        <v>0</v>
-      </c>
-      <c r="M110" s="58">
-        <v>0</v>
-      </c>
-      <c r="N110" s="58">
-        <v>0</v>
-      </c>
-      <c r="O110" s="58">
-        <v>0</v>
-      </c>
-      <c r="P110" s="22"/>
-      <c r="Q110" s="22"/>
-      <c r="R110" s="22"/>
-      <c r="S110" s="22"/>
-      <c r="T110" s="22"/>
-      <c r="U110" s="22"/>
-      <c r="V110" s="22"/>
-      <c r="W110" s="31"/>
+      <c r="L110" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="M110" s="88">
+        <v>0</v>
+      </c>
+      <c r="N110" s="88">
+        <v>0</v>
+      </c>
+      <c r="O110" s="88">
+        <v>0</v>
+      </c>
+      <c r="P110" s="66"/>
+      <c r="Q110" s="66"/>
+      <c r="R110" s="66"/>
+      <c r="S110" s="66"/>
+      <c r="T110" s="66"/>
+      <c r="U110" s="66"/>
+      <c r="V110" s="66"/>
+      <c r="W110" s="117"/>
     </row>
     <row r="111" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="32" t="s">
@@ -8189,59 +8160,59 @@
       <c r="K112" s="58">
         <v>0</v>
       </c>
-      <c r="L112" s="113">
+      <c r="L112" s="88">
         <v>0.1</v>
       </c>
-      <c r="M112" s="113">
-        <v>0</v>
-      </c>
-      <c r="N112" s="113">
-        <v>0</v>
-      </c>
-      <c r="O112" s="113">
-        <v>0</v>
-      </c>
-      <c r="P112" s="114">
-        <v>0</v>
-      </c>
-      <c r="Q112" s="114">
-        <v>0</v>
-      </c>
-      <c r="R112" s="114">
-        <v>0</v>
-      </c>
-      <c r="S112" s="114">
-        <v>0</v>
-      </c>
-      <c r="T112" s="114">
-        <v>0</v>
-      </c>
-      <c r="U112" s="114">
-        <v>0</v>
-      </c>
-      <c r="V112" s="114">
-        <v>0</v>
-      </c>
-      <c r="W112" s="115">
+      <c r="M112" s="88">
+        <v>0</v>
+      </c>
+      <c r="N112" s="88">
+        <v>0</v>
+      </c>
+      <c r="O112" s="88">
+        <v>0</v>
+      </c>
+      <c r="P112" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q112" s="89">
+        <v>0</v>
+      </c>
+      <c r="R112" s="89">
+        <v>0</v>
+      </c>
+      <c r="S112" s="89">
+        <v>0</v>
+      </c>
+      <c r="T112" s="89">
+        <v>0</v>
+      </c>
+      <c r="U112" s="89">
+        <v>0</v>
+      </c>
+      <c r="V112" s="89">
+        <v>0</v>
+      </c>
+      <c r="W112" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="99" t="s">
+      <c r="B113" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="C113" s="100"/>
-      <c r="D113" s="100"/>
-      <c r="E113" s="100"/>
-      <c r="F113" s="100"/>
-      <c r="G113" s="100"/>
+      <c r="C113" s="115"/>
+      <c r="D113" s="115"/>
+      <c r="E113" s="115"/>
+      <c r="F113" s="115"/>
+      <c r="G113" s="115"/>
       <c r="H113" s="29">
         <f t="shared" ref="H113:W113" si="2">SUM(H4:H112)</f>
         <v>36.15</v>
       </c>
       <c r="I113" s="14">
         <f t="shared" si="2"/>
-        <v>8.3149999999999977</v>
+        <v>10.244999999999999</v>
       </c>
       <c r="J113" s="12">
         <f t="shared" si="2"/>
@@ -8253,7 +8224,7 @@
       </c>
       <c r="L113" s="13">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="M113" s="15">
         <f t="shared" si="2"/>
@@ -8269,7 +8240,7 @@
       </c>
       <c r="P113" s="15">
         <f t="shared" si="2"/>
-        <v>5.6449999999999978</v>
+        <v>7.4749999999999988</v>
       </c>
       <c r="Q113" s="15">
         <f t="shared" si="2"/>
@@ -8309,22 +8280,22 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
-      <c r="J114" s="85" t="s">
+      <c r="J114" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="K114" s="86"/>
-      <c r="L114" s="86"/>
-      <c r="M114" s="86"/>
-      <c r="N114" s="86"/>
-      <c r="O114" s="86"/>
-      <c r="P114" s="86"/>
-      <c r="Q114" s="86"/>
-      <c r="R114" s="86"/>
-      <c r="S114" s="86"/>
-      <c r="T114" s="86"/>
-      <c r="U114" s="86"/>
-      <c r="V114" s="86"/>
-      <c r="W114" s="87"/>
+      <c r="K114" s="92"/>
+      <c r="L114" s="92"/>
+      <c r="M114" s="92"/>
+      <c r="N114" s="92"/>
+      <c r="O114" s="92"/>
+      <c r="P114" s="92"/>
+      <c r="Q114" s="92"/>
+      <c r="R114" s="92"/>
+      <c r="S114" s="92"/>
+      <c r="T114" s="92"/>
+      <c r="U114" s="92"/>
+      <c r="V114" s="92"/>
+      <c r="W114" s="93"/>
     </row>
     <row r="115" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="2"/>
@@ -8349,10 +8320,10 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="85" t="s">
+      <c r="H116" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="I116" s="109"/>
+      <c r="I116" s="103"/>
       <c r="J116" s="13">
         <f>H113-J113</f>
         <v>36.15</v>
@@ -8363,51 +8334,51 @@
       </c>
       <c r="L116" s="13">
         <f>K116-L113</f>
-        <v>36.049999999999997</v>
+        <v>35.949999999999996</v>
       </c>
       <c r="M116" s="13">
         <f>L116-M113</f>
-        <v>35.979999999999997</v>
+        <v>35.879999999999995</v>
       </c>
       <c r="N116" s="13">
         <f t="shared" ref="N116:W116" si="3">M116-N113</f>
-        <v>35.979999999999997</v>
+        <v>35.879999999999995</v>
       </c>
       <c r="O116" s="13">
         <f t="shared" si="3"/>
-        <v>33.479999999999997</v>
+        <v>33.379999999999995</v>
       </c>
       <c r="P116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="Q116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="R116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="S116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="T116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="U116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="V116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
       <c r="W116" s="13">
         <f t="shared" si="3"/>
-        <v>27.835000000000001</v>
+        <v>25.904999999999998</v>
       </c>
     </row>
     <row r="117" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8430,27 +8401,27 @@
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
-      <c r="H118" s="85" t="s">
+      <c r="H118" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="I118" s="86"/>
-      <c r="J118" s="85">
+      <c r="I118" s="92"/>
+      <c r="J118" s="91">
         <f>H113-I113</f>
-        <v>27.835000000000001</v>
-      </c>
-      <c r="K118" s="86"/>
-      <c r="L118" s="86"/>
-      <c r="M118" s="86"/>
-      <c r="N118" s="86"/>
-      <c r="O118" s="86"/>
-      <c r="P118" s="86"/>
-      <c r="Q118" s="86"/>
-      <c r="R118" s="86"/>
-      <c r="S118" s="86"/>
-      <c r="T118" s="86"/>
-      <c r="U118" s="86"/>
-      <c r="V118" s="86"/>
-      <c r="W118" s="87"/>
+        <v>25.905000000000001</v>
+      </c>
+      <c r="K118" s="92"/>
+      <c r="L118" s="92"/>
+      <c r="M118" s="92"/>
+      <c r="N118" s="92"/>
+      <c r="O118" s="92"/>
+      <c r="P118" s="92"/>
+      <c r="Q118" s="92"/>
+      <c r="R118" s="92"/>
+      <c r="S118" s="92"/>
+      <c r="T118" s="92"/>
+      <c r="U118" s="92"/>
+      <c r="V118" s="92"/>
+      <c r="W118" s="93"/>
     </row>
     <row r="119" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B119" s="3"/>
@@ -8538,13 +8509,6 @@
     <row r="137" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="J118:W118"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B80:B99"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="B100:B108"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="H118:I118"/>
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="J114:W114"/>
     <mergeCell ref="B16:B65"/>
@@ -8553,6 +8517,13 @@
     <mergeCell ref="B4:B11"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B113:G113"/>
+    <mergeCell ref="J118:W118"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B80:B99"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="B100:B108"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H118:I118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8566,7 +8537,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8578,7 +8549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Introducida la animación de Link cuando este sufre daño, ahora el SpriteSheet incluye las animaciones cuando link ha recibido daño
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
@@ -1304,6 +1304,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1313,9 +1322,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1342,48 +1384,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1469,22 +1469,22 @@
                   <c:v>20.567999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.997999999999998</c:v>
+                  <c:v>17.080999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.997999999999998</c:v>
+                  <c:v>17.080999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.997999999999998</c:v>
+                  <c:v>17.080999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.997999999999998</c:v>
+                  <c:v>17.080999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.997999999999998</c:v>
+                  <c:v>17.080999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.997999999999998</c:v>
+                  <c:v>17.080999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1505,11 +1505,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-198824704"/>
-        <c:axId val="-198839936"/>
+        <c:axId val="1042440816"/>
+        <c:axId val="1042434832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-198824704"/>
+        <c:axId val="1042440816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,7 +1519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-198839936"/>
+        <c:crossAx val="1042434832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1527,7 +1527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-198839936"/>
+        <c:axId val="1042434832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1538,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-198824704"/>
+        <c:crossAx val="1042440816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1580,7 +1580,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q64" sqref="Q64:W64"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R108" sqref="R108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1920,22 +1920,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="100"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="103"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="89" t="s">
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="56" t="s">
@@ -2073,8 +2073,8 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="117"/>
-      <c r="C5" s="101" t="s">
+      <c r="B5" s="110"/>
+      <c r="C5" s="112" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="77" t="s">
@@ -2140,8 +2140,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="117"/>
-      <c r="C6" s="119"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="113"/>
       <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
@@ -2205,7 +2205,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="117"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="117"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="76" t="s">
         <v>16</v>
       </c>
@@ -2335,7 +2335,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="118"/>
+      <c r="B9" s="111"/>
       <c r="C9" s="36" t="s">
         <v>109</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="114" t="s">
+      <c r="B10" s="107" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="93" t="s">
@@ -2455,7 +2455,7 @@
       <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="114"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2508,8 +2508,8 @@
       <c r="W11" s="28"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B12" s="114"/>
-      <c r="C12" s="101" t="s">
+      <c r="B12" s="107"/>
+      <c r="C12" s="112" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="49" t="s">
@@ -2563,8 +2563,8 @@
       <c r="W12" s="30"/>
     </row>
     <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="115"/>
-      <c r="C13" s="102"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="37" t="s">
         <v>117</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="W13" s="41"/>
     </row>
     <row r="14" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="104" t="s">
         <v>119</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -2683,7 +2683,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="111"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="111"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
@@ -2813,7 +2813,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="111"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
@@ -2878,7 +2878,7 @@
       </c>
     </row>
     <row r="18" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="111"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2943,7 +2943,7 @@
       </c>
     </row>
     <row r="19" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="111"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
@@ -3008,7 +3008,7 @@
       </c>
     </row>
     <row r="20" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="111"/>
+      <c r="B20" s="104"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3073,7 +3073,7 @@
       </c>
     </row>
     <row r="21" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="111"/>
+      <c r="B21" s="104"/>
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
@@ -3138,7 +3138,7 @@
       </c>
     </row>
     <row r="22" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="111"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
@@ -3203,7 +3203,7 @@
       </c>
     </row>
     <row r="23" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="111"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -3268,7 +3268,7 @@
       </c>
     </row>
     <row r="24" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="111"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
     </row>
     <row r="25" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="111"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3398,7 +3398,7 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="111"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3463,7 +3463,7 @@
       </c>
     </row>
     <row r="27" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="111"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
@@ -3528,7 +3528,7 @@
       </c>
     </row>
     <row r="28" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="111"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
@@ -3593,7 +3593,7 @@
       </c>
     </row>
     <row r="29" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="111"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
@@ -3658,7 +3658,7 @@
       </c>
     </row>
     <row r="30" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="111"/>
+      <c r="B30" s="104"/>
       <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
@@ -3723,7 +3723,7 @@
       </c>
     </row>
     <row r="31" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="111"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
@@ -3788,7 +3788,7 @@
       </c>
     </row>
     <row r="32" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="111"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3853,7 +3853,7 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="111"/>
+      <c r="B33" s="104"/>
       <c r="C33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3918,7 +3918,7 @@
       </c>
     </row>
     <row r="34" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="111"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3983,7 +3983,7 @@
       </c>
     </row>
     <row r="35" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="111"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
@@ -4048,7 +4048,7 @@
       </c>
     </row>
     <row r="36" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="111"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="4" t="s">
         <v>48</v>
       </c>
@@ -4113,7 +4113,7 @@
       </c>
     </row>
     <row r="37" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="111"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
@@ -4178,7 +4178,7 @@
       </c>
     </row>
     <row r="38" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="111"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4243,7 +4243,7 @@
       </c>
     </row>
     <row r="39" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="111"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="4" t="s">
         <v>51</v>
       </c>
@@ -4308,7 +4308,7 @@
       </c>
     </row>
     <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="111"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="4" t="s">
         <v>52</v>
       </c>
@@ -4373,7 +4373,7 @@
       </c>
     </row>
     <row r="41" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="111"/>
+      <c r="B41" s="104"/>
       <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4438,7 +4438,7 @@
       </c>
     </row>
     <row r="42" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="111"/>
+      <c r="B42" s="104"/>
       <c r="C42" s="4" t="s">
         <v>54</v>
       </c>
@@ -4503,7 +4503,7 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="111"/>
+      <c r="B43" s="104"/>
       <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
@@ -4568,7 +4568,7 @@
       </c>
     </row>
     <row r="44" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="111"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="4" t="s">
         <v>56</v>
       </c>
@@ -4633,7 +4633,7 @@
       </c>
     </row>
     <row r="45" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="111"/>
+      <c r="B45" s="104"/>
       <c r="C45" s="4" t="s">
         <v>57</v>
       </c>
@@ -4698,7 +4698,7 @@
       </c>
     </row>
     <row r="46" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="111"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
@@ -4763,7 +4763,7 @@
       </c>
     </row>
     <row r="47" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="111"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="4" t="s">
         <v>59</v>
       </c>
@@ -4828,7 +4828,7 @@
       </c>
     </row>
     <row r="48" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="111"/>
+      <c r="B48" s="104"/>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
@@ -4893,7 +4893,7 @@
       </c>
     </row>
     <row r="49" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="111"/>
+      <c r="B49" s="104"/>
       <c r="C49" s="18" t="s">
         <v>61</v>
       </c>
@@ -4958,7 +4958,7 @@
       </c>
     </row>
     <row r="50" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="111"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="18" t="s">
         <v>77</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="W50" s="28"/>
     </row>
     <row r="51" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="111"/>
+      <c r="B51" s="104"/>
       <c r="C51" s="18" t="s">
         <v>78</v>
       </c>
@@ -5064,7 +5064,7 @@
       <c r="W51" s="28"/>
     </row>
     <row r="52" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="111"/>
+      <c r="B52" s="104"/>
       <c r="C52" s="18" t="s">
         <v>79</v>
       </c>
@@ -5117,7 +5117,7 @@
       <c r="W52" s="28"/>
     </row>
     <row r="53" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="111"/>
+      <c r="B53" s="104"/>
       <c r="C53" s="18" t="s">
         <v>80</v>
       </c>
@@ -5170,7 +5170,7 @@
       <c r="W53" s="28"/>
     </row>
     <row r="54" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="111"/>
+      <c r="B54" s="104"/>
       <c r="C54" s="18" t="s">
         <v>81</v>
       </c>
@@ -5223,7 +5223,7 @@
       <c r="W54" s="28"/>
     </row>
     <row r="55" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="111"/>
+      <c r="B55" s="104"/>
       <c r="C55" s="18" t="s">
         <v>82</v>
       </c>
@@ -5276,7 +5276,7 @@
       <c r="W55" s="28"/>
     </row>
     <row r="56" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="111"/>
+      <c r="B56" s="104"/>
       <c r="C56" s="18" t="s">
         <v>83</v>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="W56" s="28"/>
     </row>
     <row r="57" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="111"/>
+      <c r="B57" s="104"/>
       <c r="C57" s="18" t="s">
         <v>84</v>
       </c>
@@ -5382,7 +5382,7 @@
       <c r="W57" s="28"/>
     </row>
     <row r="58" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="111"/>
+      <c r="B58" s="104"/>
       <c r="C58" s="18" t="s">
         <v>85</v>
       </c>
@@ -5435,7 +5435,7 @@
       <c r="W58" s="28"/>
     </row>
     <row r="59" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="111"/>
+      <c r="B59" s="104"/>
       <c r="C59" s="18" t="s">
         <v>86</v>
       </c>
@@ -5488,7 +5488,7 @@
       <c r="W59" s="28"/>
     </row>
     <row r="60" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="111"/>
+      <c r="B60" s="104"/>
       <c r="C60" s="18" t="s">
         <v>87</v>
       </c>
@@ -5541,7 +5541,7 @@
       <c r="W60" s="28"/>
     </row>
     <row r="61" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="111"/>
+      <c r="B61" s="104"/>
       <c r="C61" s="18" t="s">
         <v>88</v>
       </c>
@@ -5594,7 +5594,7 @@
       <c r="W61" s="28"/>
     </row>
     <row r="62" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="111"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="18" t="s">
         <v>89</v>
       </c>
@@ -5647,7 +5647,7 @@
       <c r="W62" s="28"/>
     </row>
     <row r="63" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="112"/>
+      <c r="B63" s="105"/>
       <c r="C63" s="36" t="s">
         <v>90</v>
       </c>
@@ -5700,7 +5700,7 @@
       <c r="W63" s="41"/>
     </row>
     <row r="64" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="113" t="s">
+      <c r="B64" s="106" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="32" t="s">
@@ -5767,7 +5767,7 @@
       </c>
     </row>
     <row r="65" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="111"/>
+      <c r="B65" s="104"/>
       <c r="C65" s="18" t="s">
         <v>64</v>
       </c>
@@ -5820,7 +5820,7 @@
       <c r="W65" s="28"/>
     </row>
     <row r="66" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="111"/>
+      <c r="B66" s="104"/>
       <c r="C66" s="18" t="s">
         <v>65</v>
       </c>
@@ -5873,7 +5873,7 @@
       <c r="W66" s="28"/>
     </row>
     <row r="67" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="111"/>
+      <c r="B67" s="104"/>
       <c r="C67" s="18" t="s">
         <v>66</v>
       </c>
@@ -5926,7 +5926,7 @@
       <c r="W67" s="28"/>
     </row>
     <row r="68" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="111"/>
+      <c r="B68" s="104"/>
       <c r="C68" s="18" t="s">
         <v>67</v>
       </c>
@@ -5979,7 +5979,7 @@
       <c r="W68" s="28"/>
     </row>
     <row r="69" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="111"/>
+      <c r="B69" s="104"/>
       <c r="C69" s="18" t="s">
         <v>68</v>
       </c>
@@ -6032,7 +6032,7 @@
       <c r="W69" s="28"/>
     </row>
     <row r="70" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="111"/>
+      <c r="B70" s="104"/>
       <c r="C70" s="18" t="s">
         <v>69</v>
       </c>
@@ -6085,7 +6085,7 @@
       <c r="W70" s="28"/>
     </row>
     <row r="71" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="111"/>
+      <c r="B71" s="104"/>
       <c r="C71" s="18" t="s">
         <v>70</v>
       </c>
@@ -6138,7 +6138,7 @@
       <c r="W71" s="28"/>
     </row>
     <row r="72" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="111"/>
+      <c r="B72" s="104"/>
       <c r="C72" s="18" t="s">
         <v>71</v>
       </c>
@@ -6191,7 +6191,7 @@
       <c r="W72" s="28"/>
     </row>
     <row r="73" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="111"/>
+      <c r="B73" s="104"/>
       <c r="C73" s="18" t="s">
         <v>72</v>
       </c>
@@ -6244,7 +6244,7 @@
       <c r="W73" s="28"/>
     </row>
     <row r="74" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="111"/>
+      <c r="B74" s="104"/>
       <c r="C74" s="18" t="s">
         <v>73</v>
       </c>
@@ -6297,7 +6297,7 @@
       <c r="W74" s="28"/>
     </row>
     <row r="75" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="111"/>
+      <c r="B75" s="104"/>
       <c r="C75" s="18" t="s">
         <v>74</v>
       </c>
@@ -6350,7 +6350,7 @@
       <c r="W75" s="28"/>
     </row>
     <row r="76" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="111"/>
+      <c r="B76" s="104"/>
       <c r="C76" s="18" t="s">
         <v>75</v>
       </c>
@@ -6403,7 +6403,7 @@
       <c r="W76" s="28"/>
     </row>
     <row r="77" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="112"/>
+      <c r="B77" s="105"/>
       <c r="C77" s="36" t="s">
         <v>76</v>
       </c>
@@ -6456,7 +6456,7 @@
       <c r="W77" s="41"/>
     </row>
     <row r="78" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="103" t="s">
+      <c r="B78" s="117" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="6" t="s">
@@ -6523,7 +6523,7 @@
       </c>
     </row>
     <row r="79" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="104"/>
+      <c r="B79" s="118"/>
       <c r="C79" s="4" t="s">
         <v>26</v>
       </c>
@@ -6588,7 +6588,7 @@
       </c>
     </row>
     <row r="80" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="104"/>
+      <c r="B80" s="118"/>
       <c r="C80" s="4" t="s">
         <v>28</v>
       </c>
@@ -6653,7 +6653,7 @@
       </c>
     </row>
     <row r="81" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="104"/>
+      <c r="B81" s="118"/>
       <c r="C81" s="4" t="s">
         <v>29</v>
       </c>
@@ -6718,7 +6718,7 @@
       </c>
     </row>
     <row r="82" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="104"/>
+      <c r="B82" s="118"/>
       <c r="C82" s="4" t="s">
         <v>30</v>
       </c>
@@ -6783,7 +6783,7 @@
       </c>
     </row>
     <row r="83" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="104"/>
+      <c r="B83" s="118"/>
       <c r="C83" s="4" t="s">
         <v>31</v>
       </c>
@@ -6848,7 +6848,7 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="104"/>
+      <c r="B84" s="118"/>
       <c r="C84" s="4" t="s">
         <v>32</v>
       </c>
@@ -6913,7 +6913,7 @@
       </c>
     </row>
     <row r="85" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="104"/>
+      <c r="B85" s="118"/>
       <c r="C85" s="4" t="s">
         <v>33</v>
       </c>
@@ -6978,7 +6978,7 @@
       </c>
     </row>
     <row r="86" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="104"/>
+      <c r="B86" s="118"/>
       <c r="C86" s="4" t="s">
         <v>34</v>
       </c>
@@ -7043,7 +7043,7 @@
       </c>
     </row>
     <row r="87" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="104"/>
+      <c r="B87" s="118"/>
       <c r="C87" s="4" t="s">
         <v>35</v>
       </c>
@@ -7108,7 +7108,7 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="104"/>
+      <c r="B88" s="118"/>
       <c r="C88" s="4" t="s">
         <v>36</v>
       </c>
@@ -7173,7 +7173,7 @@
       </c>
     </row>
     <row r="89" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="104"/>
+      <c r="B89" s="118"/>
       <c r="C89" s="4" t="s">
         <v>37</v>
       </c>
@@ -7238,7 +7238,7 @@
       </c>
     </row>
     <row r="90" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="104"/>
+      <c r="B90" s="118"/>
       <c r="C90" s="4" t="s">
         <v>38</v>
       </c>
@@ -7303,7 +7303,7 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="104"/>
+      <c r="B91" s="118"/>
       <c r="C91" s="4" t="s">
         <v>39</v>
       </c>
@@ -7368,7 +7368,7 @@
       </c>
     </row>
     <row r="92" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="104"/>
+      <c r="B92" s="118"/>
       <c r="C92" s="4" t="s">
         <v>40</v>
       </c>
@@ -7433,7 +7433,7 @@
       </c>
     </row>
     <row r="93" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="104"/>
+      <c r="B93" s="118"/>
       <c r="C93" s="4" t="s">
         <v>41</v>
       </c>
@@ -7498,7 +7498,7 @@
       </c>
     </row>
     <row r="94" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="104"/>
+      <c r="B94" s="118"/>
       <c r="C94" s="4" t="s">
         <v>120</v>
       </c>
@@ -7563,7 +7563,7 @@
       </c>
     </row>
     <row r="95" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="104"/>
+      <c r="B95" s="118"/>
       <c r="C95" s="4" t="s">
         <v>121</v>
       </c>
@@ -7628,7 +7628,7 @@
       </c>
     </row>
     <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="104"/>
+      <c r="B96" s="118"/>
       <c r="C96" s="4" t="s">
         <v>42</v>
       </c>
@@ -7693,7 +7693,7 @@
       </c>
     </row>
     <row r="97" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="105"/>
+      <c r="B97" s="119"/>
       <c r="C97" s="36" t="s">
         <v>92</v>
       </c>
@@ -7746,10 +7746,10 @@
       <c r="W97" s="41"/>
     </row>
     <row r="98" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="108" t="s">
+      <c r="B98" s="122" t="s">
         <v>93</v>
       </c>
-      <c r="C98" s="106" t="s">
+      <c r="C98" s="120" t="s">
         <v>94</v>
       </c>
       <c r="D98" s="6" t="s">
@@ -7815,8 +7815,8 @@
       </c>
     </row>
     <row r="99" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="108"/>
-      <c r="C99" s="107"/>
+      <c r="B99" s="122"/>
+      <c r="C99" s="121"/>
       <c r="D99" s="4" t="s">
         <v>96</v>
       </c>
@@ -7880,8 +7880,8 @@
       </c>
     </row>
     <row r="100" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="108"/>
-      <c r="C100" s="107"/>
+      <c r="B100" s="122"/>
+      <c r="C100" s="121"/>
       <c r="D100" s="4" t="s">
         <v>97</v>
       </c>
@@ -7899,7 +7899,7 @@
       </c>
       <c r="I100" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="J100" s="50">
         <v>0</v>
@@ -7925,15 +7925,27 @@
       <c r="Q100" s="50">
         <v>0</v>
       </c>
-      <c r="R100" s="122"/>
-      <c r="S100" s="122"/>
-      <c r="T100" s="122"/>
-      <c r="U100" s="122"/>
-      <c r="V100" s="122"/>
-      <c r="W100" s="123"/>
+      <c r="R100" s="67">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="S100" s="70">
+        <v>0</v>
+      </c>
+      <c r="T100" s="70">
+        <v>0</v>
+      </c>
+      <c r="U100" s="70">
+        <v>0</v>
+      </c>
+      <c r="V100" s="70">
+        <v>0</v>
+      </c>
+      <c r="W100" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="108"/>
+      <c r="B101" s="122"/>
       <c r="C101" s="18" t="s">
         <v>115</v>
       </c>
@@ -7978,15 +7990,15 @@
       <c r="Q101" s="50">
         <v>0</v>
       </c>
-      <c r="R101" s="122"/>
-      <c r="S101" s="122"/>
-      <c r="T101" s="122"/>
-      <c r="U101" s="122"/>
-      <c r="V101" s="122"/>
-      <c r="W101" s="123"/>
+      <c r="R101" s="98"/>
+      <c r="S101" s="98"/>
+      <c r="T101" s="98"/>
+      <c r="U101" s="98"/>
+      <c r="V101" s="98"/>
+      <c r="W101" s="99"/>
     </row>
     <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="108"/>
+      <c r="B102" s="122"/>
       <c r="C102" s="18" t="s">
         <v>98</v>
       </c>
@@ -8031,15 +8043,15 @@
       <c r="Q102" s="50">
         <v>0</v>
       </c>
-      <c r="R102" s="122"/>
-      <c r="S102" s="122"/>
-      <c r="T102" s="122"/>
-      <c r="U102" s="122"/>
-      <c r="V102" s="122"/>
-      <c r="W102" s="123"/>
+      <c r="R102" s="98"/>
+      <c r="S102" s="98"/>
+      <c r="T102" s="98"/>
+      <c r="U102" s="98"/>
+      <c r="V102" s="98"/>
+      <c r="W102" s="99"/>
     </row>
     <row r="103" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="108"/>
+      <c r="B103" s="122"/>
       <c r="C103" s="18" t="s">
         <v>99</v>
       </c>
@@ -8084,15 +8096,15 @@
       <c r="Q103" s="50">
         <v>0</v>
       </c>
-      <c r="R103" s="124"/>
-      <c r="S103" s="122"/>
-      <c r="T103" s="122"/>
-      <c r="U103" s="122"/>
-      <c r="V103" s="122"/>
-      <c r="W103" s="123"/>
+      <c r="R103" s="100"/>
+      <c r="S103" s="98"/>
+      <c r="T103" s="98"/>
+      <c r="U103" s="98"/>
+      <c r="V103" s="98"/>
+      <c r="W103" s="99"/>
     </row>
     <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="108"/>
+      <c r="B104" s="122"/>
       <c r="C104" s="18" t="s">
         <v>100</v>
       </c>
@@ -8157,7 +8169,7 @@
       </c>
     </row>
     <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="108"/>
+      <c r="B105" s="122"/>
       <c r="C105" s="18" t="s">
         <v>101</v>
       </c>
@@ -8202,15 +8214,15 @@
       <c r="Q105" s="50">
         <v>0</v>
       </c>
-      <c r="R105" s="122"/>
-      <c r="S105" s="122"/>
-      <c r="T105" s="122"/>
-      <c r="U105" s="122"/>
-      <c r="V105" s="122"/>
-      <c r="W105" s="123"/>
+      <c r="R105" s="98"/>
+      <c r="S105" s="98"/>
+      <c r="T105" s="98"/>
+      <c r="U105" s="98"/>
+      <c r="V105" s="98"/>
+      <c r="W105" s="99"/>
     </row>
     <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="109"/>
+      <c r="B106" s="123"/>
       <c r="C106" s="18" t="s">
         <v>102</v>
       </c>
@@ -8497,21 +8509,21 @@
       </c>
     </row>
     <row r="111" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="120" t="s">
+      <c r="B111" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="C111" s="121"/>
-      <c r="D111" s="121"/>
-      <c r="E111" s="121"/>
-      <c r="F111" s="121"/>
-      <c r="G111" s="121"/>
+      <c r="C111" s="115"/>
+      <c r="D111" s="115"/>
+      <c r="E111" s="115"/>
+      <c r="F111" s="115"/>
+      <c r="G111" s="115"/>
       <c r="H111" s="27">
         <f t="shared" ref="H111:W111" si="2">SUM(H4:H110)</f>
         <v>35.800000000000004</v>
       </c>
       <c r="I111" s="14">
         <f t="shared" si="2"/>
-        <v>17.801999999999996</v>
+        <v>18.718999999999998</v>
       </c>
       <c r="J111" s="12">
         <f t="shared" si="2"/>
@@ -8547,7 +8559,7 @@
       </c>
       <c r="R111" s="15">
         <f t="shared" si="2"/>
-        <v>2.57</v>
+        <v>3.4870000000000001</v>
       </c>
       <c r="S111" s="15">
         <f t="shared" si="2"/>
@@ -8579,22 +8591,22 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
-      <c r="J112" s="98" t="s">
+      <c r="J112" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="K112" s="99"/>
-      <c r="L112" s="99"/>
-      <c r="M112" s="99"/>
-      <c r="N112" s="99"/>
-      <c r="O112" s="99"/>
-      <c r="P112" s="99"/>
-      <c r="Q112" s="99"/>
-      <c r="R112" s="99"/>
-      <c r="S112" s="99"/>
-      <c r="T112" s="99"/>
-      <c r="U112" s="99"/>
-      <c r="V112" s="99"/>
-      <c r="W112" s="100"/>
+      <c r="K112" s="102"/>
+      <c r="L112" s="102"/>
+      <c r="M112" s="102"/>
+      <c r="N112" s="102"/>
+      <c r="O112" s="102"/>
+      <c r="P112" s="102"/>
+      <c r="Q112" s="102"/>
+      <c r="R112" s="102"/>
+      <c r="S112" s="102"/>
+      <c r="T112" s="102"/>
+      <c r="U112" s="102"/>
+      <c r="V112" s="102"/>
+      <c r="W112" s="103"/>
     </row>
     <row r="113" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="2"/>
@@ -8619,10 +8631,10 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="98" t="s">
+      <c r="H114" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="I114" s="110"/>
+      <c r="I114" s="124"/>
       <c r="J114" s="13">
         <f>H111-J111</f>
         <v>35.800000000000004</v>
@@ -8657,27 +8669,27 @@
       </c>
       <c r="R114" s="13">
         <f t="shared" si="3"/>
-        <v>17.997999999999998</v>
+        <v>17.080999999999996</v>
       </c>
       <c r="S114" s="13">
         <f t="shared" si="3"/>
-        <v>17.997999999999998</v>
+        <v>17.080999999999996</v>
       </c>
       <c r="T114" s="13">
         <f t="shared" si="3"/>
-        <v>17.997999999999998</v>
+        <v>17.080999999999996</v>
       </c>
       <c r="U114" s="13">
         <f t="shared" si="3"/>
-        <v>17.997999999999998</v>
+        <v>17.080999999999996</v>
       </c>
       <c r="V114" s="13">
         <f t="shared" si="3"/>
-        <v>17.997999999999998</v>
+        <v>17.080999999999996</v>
       </c>
       <c r="W114" s="13">
         <f t="shared" si="3"/>
-        <v>17.997999999999998</v>
+        <v>17.080999999999996</v>
       </c>
     </row>
     <row r="115" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8700,27 +8712,27 @@
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="H116" s="98" t="s">
+      <c r="H116" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="I116" s="99"/>
-      <c r="J116" s="98">
+      <c r="I116" s="102"/>
+      <c r="J116" s="101">
         <f>H111-I111</f>
-        <v>17.998000000000008</v>
-      </c>
-      <c r="K116" s="99"/>
-      <c r="L116" s="99"/>
-      <c r="M116" s="99"/>
-      <c r="N116" s="99"/>
-      <c r="O116" s="99"/>
-      <c r="P116" s="99"/>
-      <c r="Q116" s="99"/>
-      <c r="R116" s="99"/>
-      <c r="S116" s="99"/>
-      <c r="T116" s="99"/>
-      <c r="U116" s="99"/>
-      <c r="V116" s="99"/>
-      <c r="W116" s="100"/>
+        <v>17.081000000000007</v>
+      </c>
+      <c r="K116" s="102"/>
+      <c r="L116" s="102"/>
+      <c r="M116" s="102"/>
+      <c r="N116" s="102"/>
+      <c r="O116" s="102"/>
+      <c r="P116" s="102"/>
+      <c r="Q116" s="102"/>
+      <c r="R116" s="102"/>
+      <c r="S116" s="102"/>
+      <c r="T116" s="102"/>
+      <c r="U116" s="102"/>
+      <c r="V116" s="102"/>
+      <c r="W116" s="103"/>
     </row>
     <row r="117" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B117" s="3"/>
@@ -8808,6 +8820,13 @@
     <row r="135" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J116:W116"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B78:B97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="B98:B106"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H116:I116"/>
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="J112:W112"/>
     <mergeCell ref="B14:B63"/>
@@ -8816,13 +8835,6 @@
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B111:G111"/>
-    <mergeCell ref="J116:W116"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B78:B97"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="B98:B106"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H116:I116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ahora solo puede haber una flecha a la vez, y unicamente si Link ataca teniendo toda la vida
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devildrake\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -392,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1310,7 +1310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1322,9 +1322,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1352,40 +1385,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1406,7 +1406,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1472,28 +1472,28 @@
                   <c:v>20.567999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.920999999999999</c:v>
+                  <c:v>16.160999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.920999999999999</c:v>
+                  <c:v>16.160999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.920999999999999</c:v>
+                  <c:v>16.160999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.920999999999999</c:v>
+                  <c:v>16.160999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.920999999999999</c:v>
+                  <c:v>16.160999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.920999999999999</c:v>
+                  <c:v>16.160999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-08BE-4709-9DE4-AEC2E98B8D97}"/>
             </c:ext>
@@ -1508,11 +1508,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1042440816"/>
-        <c:axId val="1042434832"/>
+        <c:axId val="-349567968"/>
+        <c:axId val="-349567424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1042440816"/>
+        <c:axId val="-349567968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1042434832"/>
+        <c:crossAx val="-349567424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1530,7 +1530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1042434832"/>
+        <c:axId val="-349567424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1541,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1042440816"/>
+        <c:crossAx val="-349567968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1583,7 +1583,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1893,28 +1893,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R69" sqref="R69"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R104" sqref="R104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>118</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J2" s="101" t="s">
         <v>5</v>
       </c>
@@ -1940,7 +1940,7 @@
       <c r="V2" s="102"/>
       <c r="W2" s="103"/>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="89" t="s">
         <v>7</v>
       </c>
@@ -2008,8 +2008,8 @@
         <v>43053</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="119" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="56" t="s">
@@ -2075,9 +2075,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="120"/>
-      <c r="C5" s="104" t="s">
+    <row r="5" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="110"/>
+      <c r="C5" s="112" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="77" t="s">
@@ -2142,9 +2142,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="120"/>
-      <c r="C6" s="122"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="110"/>
+      <c r="C6" s="113"/>
       <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
@@ -2207,8 +2207,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="120"/>
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="110"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2272,8 +2272,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="120"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="110"/>
       <c r="C8" s="76" t="s">
         <v>16</v>
       </c>
@@ -2337,8 +2337,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="121"/>
+    <row r="9" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="111"/>
       <c r="C9" s="36" t="s">
         <v>109</v>
       </c>
@@ -2402,8 +2402,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="117" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B10" s="107" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="93" t="s">
@@ -2457,8 +2457,8 @@
       <c r="V10" s="34"/>
       <c r="W10" s="35"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="117"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B11" s="107"/>
       <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2510,9 +2510,9 @@
       <c r="V11" s="20"/>
       <c r="W11" s="28"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="117"/>
-      <c r="C12" s="104" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B12" s="107"/>
+      <c r="C12" s="112" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="49" t="s">
@@ -2565,9 +2565,9 @@
       <c r="V12" s="23"/>
       <c r="W12" s="30"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="118"/>
-      <c r="C13" s="105"/>
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="108"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="37" t="s">
         <v>117</v>
       </c>
@@ -2618,8 +2618,8 @@
       <c r="V13" s="40"/>
       <c r="W13" s="41"/>
     </row>
-    <row r="14" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="114" t="s">
+    <row r="14" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="104" t="s">
         <v>119</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -2685,8 +2685,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="114"/>
+    <row r="15" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="104"/>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2750,8 +2750,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="114"/>
+    <row r="16" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="104"/>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
@@ -2815,8 +2815,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="114"/>
+    <row r="17" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="104"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
@@ -2880,8 +2880,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="114"/>
+    <row r="18" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="104"/>
       <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2945,8 +2945,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="114"/>
+    <row r="19" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="104"/>
       <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
@@ -3010,8 +3010,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="114"/>
+    <row r="20" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="104"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3075,8 +3075,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="114"/>
+    <row r="21" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="104"/>
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
@@ -3140,8 +3140,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="114"/>
+    <row r="22" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="104"/>
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
@@ -3205,8 +3205,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="114"/>
+    <row r="23" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="104"/>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -3270,8 +3270,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="114"/>
+    <row r="24" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="104"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
@@ -3335,8 +3335,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="114"/>
+    <row r="25" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="104"/>
       <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3400,8 +3400,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="114"/>
+    <row r="26" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="104"/>
       <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3465,8 +3465,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="114"/>
+    <row r="27" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="104"/>
       <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
@@ -3530,8 +3530,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="114"/>
+    <row r="28" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="104"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
@@ -3595,8 +3595,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="114"/>
+    <row r="29" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="104"/>
       <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
@@ -3660,8 +3660,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="114"/>
+    <row r="30" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="104"/>
       <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
@@ -3725,8 +3725,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="114"/>
+    <row r="31" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="104"/>
       <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
@@ -3790,8 +3790,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="114"/>
+    <row r="32" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="104"/>
       <c r="C32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3855,8 +3855,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="114"/>
+    <row r="33" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="104"/>
       <c r="C33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3920,8 +3920,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="114"/>
+    <row r="34" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="104"/>
       <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3985,8 +3985,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="114"/>
+    <row r="35" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="104"/>
       <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
@@ -4050,8 +4050,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="114"/>
+    <row r="36" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="104"/>
       <c r="C36" s="4" t="s">
         <v>48</v>
       </c>
@@ -4115,8 +4115,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="114"/>
+    <row r="37" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="104"/>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
@@ -4180,8 +4180,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="114"/>
+    <row r="38" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="104"/>
       <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4245,8 +4245,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="114"/>
+    <row r="39" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="104"/>
       <c r="C39" s="4" t="s">
         <v>51</v>
       </c>
@@ -4310,8 +4310,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="114"/>
+    <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="104"/>
       <c r="C40" s="4" t="s">
         <v>52</v>
       </c>
@@ -4375,8 +4375,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="114"/>
+    <row r="41" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="104"/>
       <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4440,8 +4440,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="114"/>
+    <row r="42" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="104"/>
       <c r="C42" s="4" t="s">
         <v>54</v>
       </c>
@@ -4505,8 +4505,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="114"/>
+    <row r="43" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="104"/>
       <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
@@ -4570,8 +4570,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="114"/>
+    <row r="44" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="104"/>
       <c r="C44" s="4" t="s">
         <v>56</v>
       </c>
@@ -4635,8 +4635,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="114"/>
+    <row r="45" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="104"/>
       <c r="C45" s="4" t="s">
         <v>57</v>
       </c>
@@ -4700,8 +4700,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="114"/>
+    <row r="46" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="104"/>
       <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
@@ -4765,8 +4765,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="114"/>
+    <row r="47" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="104"/>
       <c r="C47" s="4" t="s">
         <v>59</v>
       </c>
@@ -4830,8 +4830,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="114"/>
+    <row r="48" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="104"/>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
@@ -4895,8 +4895,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="114"/>
+    <row r="49" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="104"/>
       <c r="C49" s="18" t="s">
         <v>61</v>
       </c>
@@ -4960,8 +4960,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="114"/>
+    <row r="50" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="104"/>
       <c r="C50" s="18" t="s">
         <v>77</v>
       </c>
@@ -5013,8 +5013,8 @@
       <c r="V50" s="20"/>
       <c r="W50" s="28"/>
     </row>
-    <row r="51" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="114"/>
+    <row r="51" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="104"/>
       <c r="C51" s="18" t="s">
         <v>78</v>
       </c>
@@ -5066,8 +5066,8 @@
       <c r="V51" s="20"/>
       <c r="W51" s="28"/>
     </row>
-    <row r="52" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="114"/>
+    <row r="52" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="104"/>
       <c r="C52" s="18" t="s">
         <v>79</v>
       </c>
@@ -5119,8 +5119,8 @@
       <c r="V52" s="20"/>
       <c r="W52" s="28"/>
     </row>
-    <row r="53" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="114"/>
+    <row r="53" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="104"/>
       <c r="C53" s="18" t="s">
         <v>80</v>
       </c>
@@ -5172,8 +5172,8 @@
       <c r="V53" s="20"/>
       <c r="W53" s="28"/>
     </row>
-    <row r="54" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="114"/>
+    <row r="54" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="104"/>
       <c r="C54" s="18" t="s">
         <v>81</v>
       </c>
@@ -5225,8 +5225,8 @@
       <c r="V54" s="20"/>
       <c r="W54" s="28"/>
     </row>
-    <row r="55" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="114"/>
+    <row r="55" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="104"/>
       <c r="C55" s="18" t="s">
         <v>82</v>
       </c>
@@ -5278,8 +5278,8 @@
       <c r="V55" s="20"/>
       <c r="W55" s="28"/>
     </row>
-    <row r="56" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="114"/>
+    <row r="56" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="104"/>
       <c r="C56" s="18" t="s">
         <v>83</v>
       </c>
@@ -5331,8 +5331,8 @@
       <c r="V56" s="20"/>
       <c r="W56" s="28"/>
     </row>
-    <row r="57" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="114"/>
+    <row r="57" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="104"/>
       <c r="C57" s="18" t="s">
         <v>84</v>
       </c>
@@ -5384,8 +5384,8 @@
       <c r="V57" s="20"/>
       <c r="W57" s="28"/>
     </row>
-    <row r="58" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="114"/>
+    <row r="58" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="104"/>
       <c r="C58" s="18" t="s">
         <v>85</v>
       </c>
@@ -5437,8 +5437,8 @@
       <c r="V58" s="20"/>
       <c r="W58" s="28"/>
     </row>
-    <row r="59" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="114"/>
+    <row r="59" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="104"/>
       <c r="C59" s="18" t="s">
         <v>86</v>
       </c>
@@ -5490,8 +5490,8 @@
       <c r="V59" s="20"/>
       <c r="W59" s="28"/>
     </row>
-    <row r="60" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="114"/>
+    <row r="60" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="104"/>
       <c r="C60" s="18" t="s">
         <v>87</v>
       </c>
@@ -5543,8 +5543,8 @@
       <c r="V60" s="20"/>
       <c r="W60" s="28"/>
     </row>
-    <row r="61" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="114"/>
+    <row r="61" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="104"/>
       <c r="C61" s="18" t="s">
         <v>88</v>
       </c>
@@ -5596,8 +5596,8 @@
       <c r="V61" s="20"/>
       <c r="W61" s="28"/>
     </row>
-    <row r="62" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="114"/>
+    <row r="62" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="104"/>
       <c r="C62" s="18" t="s">
         <v>89</v>
       </c>
@@ -5649,8 +5649,8 @@
       <c r="V62" s="20"/>
       <c r="W62" s="28"/>
     </row>
-    <row r="63" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="115"/>
+    <row r="63" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="105"/>
       <c r="C63" s="36" t="s">
         <v>90</v>
       </c>
@@ -5702,8 +5702,8 @@
       <c r="V63" s="40"/>
       <c r="W63" s="41"/>
     </row>
-    <row r="64" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="116" t="s">
+    <row r="64" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="106" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="32" t="s">
@@ -5744,7 +5744,7 @@
       <c r="O64" s="52">
         <v>0</v>
       </c>
-      <c r="P64" s="66">
+      <c r="P64" s="70">
         <v>1.83</v>
       </c>
       <c r="Q64" s="70">
@@ -5769,8 +5769,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="114"/>
+    <row r="65" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="104"/>
       <c r="C65" s="18" t="s">
         <v>64</v>
       </c>
@@ -5815,7 +5815,7 @@
       <c r="Q65" s="50">
         <v>0</v>
       </c>
-      <c r="R65" s="125">
+      <c r="R65" s="100">
         <v>0.16</v>
       </c>
       <c r="S65" s="20"/>
@@ -5824,8 +5824,8 @@
       <c r="V65" s="20"/>
       <c r="W65" s="28"/>
     </row>
-    <row r="66" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="114"/>
+    <row r="66" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="104"/>
       <c r="C66" s="18" t="s">
         <v>65</v>
       </c>
@@ -5877,8 +5877,8 @@
       <c r="V66" s="20"/>
       <c r="W66" s="28"/>
     </row>
-    <row r="67" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="114"/>
+    <row r="67" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="104"/>
       <c r="C67" s="18" t="s">
         <v>66</v>
       </c>
@@ -5930,8 +5930,8 @@
       <c r="V67" s="20"/>
       <c r="W67" s="28"/>
     </row>
-    <row r="68" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="114"/>
+    <row r="68" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="104"/>
       <c r="C68" s="18" t="s">
         <v>67</v>
       </c>
@@ -5983,8 +5983,8 @@
       <c r="V68" s="20"/>
       <c r="W68" s="28"/>
     </row>
-    <row r="69" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="114"/>
+    <row r="69" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="104"/>
       <c r="C69" s="18" t="s">
         <v>68</v>
       </c>
@@ -6036,8 +6036,8 @@
       <c r="V69" s="20"/>
       <c r="W69" s="28"/>
     </row>
-    <row r="70" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="114"/>
+    <row r="70" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="104"/>
       <c r="C70" s="18" t="s">
         <v>69</v>
       </c>
@@ -6089,8 +6089,8 @@
       <c r="V70" s="20"/>
       <c r="W70" s="28"/>
     </row>
-    <row r="71" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="114"/>
+    <row r="71" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="104"/>
       <c r="C71" s="18" t="s">
         <v>70</v>
       </c>
@@ -6142,8 +6142,8 @@
       <c r="V71" s="20"/>
       <c r="W71" s="28"/>
     </row>
-    <row r="72" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="114"/>
+    <row r="72" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="104"/>
       <c r="C72" s="18" t="s">
         <v>71</v>
       </c>
@@ -6195,8 +6195,8 @@
       <c r="V72" s="20"/>
       <c r="W72" s="28"/>
     </row>
-    <row r="73" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="114"/>
+    <row r="73" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="104"/>
       <c r="C73" s="18" t="s">
         <v>72</v>
       </c>
@@ -6248,8 +6248,8 @@
       <c r="V73" s="20"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="114"/>
+    <row r="74" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="104"/>
       <c r="C74" s="18" t="s">
         <v>73</v>
       </c>
@@ -6301,8 +6301,8 @@
       <c r="V74" s="20"/>
       <c r="W74" s="28"/>
     </row>
-    <row r="75" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="114"/>
+    <row r="75" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="104"/>
       <c r="C75" s="18" t="s">
         <v>74</v>
       </c>
@@ -6354,8 +6354,8 @@
       <c r="V75" s="20"/>
       <c r="W75" s="28"/>
     </row>
-    <row r="76" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="114"/>
+    <row r="76" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="104"/>
       <c r="C76" s="18" t="s">
         <v>75</v>
       </c>
@@ -6407,8 +6407,8 @@
       <c r="V76" s="20"/>
       <c r="W76" s="28"/>
     </row>
-    <row r="77" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="115"/>
+    <row r="77" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="105"/>
       <c r="C77" s="36" t="s">
         <v>76</v>
       </c>
@@ -6460,8 +6460,8 @@
       <c r="V77" s="40"/>
       <c r="W77" s="41"/>
     </row>
-    <row r="78" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="106" t="s">
+    <row r="78" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="117" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="6" t="s">
@@ -6527,8 +6527,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="107"/>
+    <row r="79" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="118"/>
       <c r="C79" s="4" t="s">
         <v>26</v>
       </c>
@@ -6592,8 +6592,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="107"/>
+    <row r="80" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B80" s="118"/>
       <c r="C80" s="4" t="s">
         <v>28</v>
       </c>
@@ -6657,8 +6657,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="107"/>
+    <row r="81" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="118"/>
       <c r="C81" s="4" t="s">
         <v>29</v>
       </c>
@@ -6722,8 +6722,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="107"/>
+    <row r="82" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B82" s="118"/>
       <c r="C82" s="4" t="s">
         <v>30</v>
       </c>
@@ -6787,8 +6787,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="107"/>
+    <row r="83" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="118"/>
       <c r="C83" s="4" t="s">
         <v>31</v>
       </c>
@@ -6852,8 +6852,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="107"/>
+    <row r="84" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="118"/>
       <c r="C84" s="4" t="s">
         <v>32</v>
       </c>
@@ -6917,8 +6917,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="107"/>
+    <row r="85" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="118"/>
       <c r="C85" s="4" t="s">
         <v>33</v>
       </c>
@@ -6982,8 +6982,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="107"/>
+    <row r="86" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="118"/>
       <c r="C86" s="4" t="s">
         <v>34</v>
       </c>
@@ -7047,8 +7047,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="107"/>
+    <row r="87" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="118"/>
       <c r="C87" s="4" t="s">
         <v>35</v>
       </c>
@@ -7112,8 +7112,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="107"/>
+    <row r="88" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="118"/>
       <c r="C88" s="4" t="s">
         <v>36</v>
       </c>
@@ -7177,8 +7177,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="107"/>
+    <row r="89" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="118"/>
       <c r="C89" s="4" t="s">
         <v>37</v>
       </c>
@@ -7242,8 +7242,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="107"/>
+    <row r="90" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="118"/>
       <c r="C90" s="4" t="s">
         <v>38</v>
       </c>
@@ -7307,8 +7307,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="107"/>
+    <row r="91" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="118"/>
       <c r="C91" s="4" t="s">
         <v>39</v>
       </c>
@@ -7372,8 +7372,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="107"/>
+    <row r="92" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="118"/>
       <c r="C92" s="4" t="s">
         <v>40</v>
       </c>
@@ -7437,8 +7437,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="107"/>
+    <row r="93" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="118"/>
       <c r="C93" s="4" t="s">
         <v>41</v>
       </c>
@@ -7502,8 +7502,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="107"/>
+    <row r="94" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="118"/>
       <c r="C94" s="4" t="s">
         <v>120</v>
       </c>
@@ -7567,8 +7567,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="107"/>
+    <row r="95" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="118"/>
       <c r="C95" s="4" t="s">
         <v>121</v>
       </c>
@@ -7632,8 +7632,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="107"/>
+    <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="118"/>
       <c r="C96" s="4" t="s">
         <v>42</v>
       </c>
@@ -7697,8 +7697,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="108"/>
+    <row r="97" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="119"/>
       <c r="C97" s="36" t="s">
         <v>92</v>
       </c>
@@ -7750,11 +7750,11 @@
       <c r="V97" s="40"/>
       <c r="W97" s="41"/>
     </row>
-    <row r="98" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="111" t="s">
+    <row r="98" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="122" t="s">
         <v>93</v>
       </c>
-      <c r="C98" s="109" t="s">
+      <c r="C98" s="120" t="s">
         <v>94</v>
       </c>
       <c r="D98" s="6" t="s">
@@ -7819,9 +7819,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="111"/>
-      <c r="C99" s="110"/>
+    <row r="99" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="122"/>
+      <c r="C99" s="121"/>
       <c r="D99" s="4" t="s">
         <v>96</v>
       </c>
@@ -7884,9 +7884,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="111"/>
-      <c r="C100" s="110"/>
+    <row r="100" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="122"/>
+      <c r="C100" s="121"/>
       <c r="D100" s="4" t="s">
         <v>97</v>
       </c>
@@ -7949,8 +7949,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="111"/>
+    <row r="101" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="122"/>
       <c r="C101" s="18" t="s">
         <v>115</v>
       </c>
@@ -8002,8 +8002,8 @@
       <c r="V101" s="98"/>
       <c r="W101" s="99"/>
     </row>
-    <row r="102" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="111"/>
+    <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="122"/>
       <c r="C102" s="18" t="s">
         <v>98</v>
       </c>
@@ -8055,8 +8055,8 @@
       <c r="V102" s="98"/>
       <c r="W102" s="99"/>
     </row>
-    <row r="103" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="111"/>
+    <row r="103" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="122"/>
       <c r="C103" s="18" t="s">
         <v>99</v>
       </c>
@@ -8075,7 +8075,7 @@
       </c>
       <c r="I103" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="J103" s="50">
         <v>0</v>
@@ -8101,15 +8101,17 @@
       <c r="Q103" s="50">
         <v>0</v>
       </c>
-      <c r="R103" s="100"/>
+      <c r="R103" s="125">
+        <v>0.76</v>
+      </c>
       <c r="S103" s="98"/>
       <c r="T103" s="98"/>
       <c r="U103" s="98"/>
       <c r="V103" s="98"/>
       <c r="W103" s="99"/>
     </row>
-    <row r="104" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="111"/>
+    <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="122"/>
       <c r="C104" s="18" t="s">
         <v>100</v>
       </c>
@@ -8173,8 +8175,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="111"/>
+    <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="122"/>
       <c r="C105" s="18" t="s">
         <v>101</v>
       </c>
@@ -8226,8 +8228,8 @@
       <c r="V105" s="98"/>
       <c r="W105" s="99"/>
     </row>
-    <row r="106" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="112"/>
+    <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="123"/>
       <c r="C106" s="18" t="s">
         <v>102</v>
       </c>
@@ -8279,7 +8281,7 @@
       <c r="V106" s="20"/>
       <c r="W106" s="28"/>
     </row>
-    <row r="107" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="29" t="s">
         <v>103</v>
       </c>
@@ -8334,7 +8336,7 @@
       <c r="V107" s="20"/>
       <c r="W107" s="28"/>
     </row>
-    <row r="108" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="29" t="s">
         <v>111</v>
       </c>
@@ -8383,7 +8385,7 @@
       <c r="V108" s="55"/>
       <c r="W108" s="74"/>
     </row>
-    <row r="109" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B109" s="29" t="s">
         <v>112</v>
       </c>
@@ -8448,7 +8450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B110" s="19" t="s">
         <v>113</v>
       </c>
@@ -8513,22 +8515,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="123" t="s">
+    <row r="111" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="C111" s="124"/>
-      <c r="D111" s="124"/>
-      <c r="E111" s="124"/>
-      <c r="F111" s="124"/>
-      <c r="G111" s="124"/>
+      <c r="C111" s="115"/>
+      <c r="D111" s="115"/>
+      <c r="E111" s="115"/>
+      <c r="F111" s="115"/>
+      <c r="G111" s="115"/>
       <c r="H111" s="27">
         <f t="shared" ref="H111:W111" si="2">SUM(H4:H110)</f>
         <v>35.800000000000004</v>
       </c>
       <c r="I111" s="14">
         <f t="shared" si="2"/>
-        <v>18.878999999999998</v>
+        <v>19.638999999999999</v>
       </c>
       <c r="J111" s="12">
         <f t="shared" si="2"/>
@@ -8564,7 +8566,7 @@
       </c>
       <c r="R111" s="15">
         <f t="shared" si="2"/>
-        <v>3.6470000000000002</v>
+        <v>4.407</v>
       </c>
       <c r="S111" s="15">
         <f t="shared" si="2"/>
@@ -8587,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -8613,7 +8615,7 @@
       <c r="V112" s="102"/>
       <c r="W112" s="103"/>
     </row>
-    <row r="113" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -8629,7 +8631,7 @@
       <c r="O113" s="11"/>
       <c r="P113" s="11"/>
     </row>
-    <row r="114" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -8639,7 +8641,7 @@
       <c r="H114" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="I114" s="113"/>
+      <c r="I114" s="124"/>
       <c r="J114" s="13">
         <f>H111-J111</f>
         <v>35.800000000000004</v>
@@ -8674,30 +8676,30 @@
       </c>
       <c r="R114" s="13">
         <f t="shared" si="3"/>
-        <v>16.920999999999999</v>
+        <v>16.160999999999998</v>
       </c>
       <c r="S114" s="13">
         <f t="shared" si="3"/>
-        <v>16.920999999999999</v>
+        <v>16.160999999999998</v>
       </c>
       <c r="T114" s="13">
         <f t="shared" si="3"/>
-        <v>16.920999999999999</v>
+        <v>16.160999999999998</v>
       </c>
       <c r="U114" s="13">
         <f t="shared" si="3"/>
-        <v>16.920999999999999</v>
+        <v>16.160999999999998</v>
       </c>
       <c r="V114" s="13">
         <f t="shared" si="3"/>
-        <v>16.920999999999999</v>
+        <v>16.160999999999998</v>
       </c>
       <c r="W114" s="13">
         <f t="shared" si="3"/>
-        <v>16.920999999999999</v>
-      </c>
-    </row>
-    <row r="115" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16.160999999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -8711,7 +8713,7 @@
       <c r="L115" s="3"/>
       <c r="M115" s="3"/>
     </row>
-    <row r="116" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
@@ -8723,7 +8725,7 @@
       <c r="I116" s="102"/>
       <c r="J116" s="101">
         <f>H111-I111</f>
-        <v>16.921000000000006</v>
+        <v>16.161000000000005</v>
       </c>
       <c r="K116" s="102"/>
       <c r="L116" s="102"/>
@@ -8739,7 +8741,7 @@
       <c r="V116" s="102"/>
       <c r="W116" s="103"/>
     </row>
-    <row r="117" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -8753,7 +8755,7 @@
       <c r="L117" s="3"/>
       <c r="M117" s="3"/>
     </row>
-    <row r="118" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
@@ -8767,7 +8769,7 @@
       <c r="L118" s="3"/>
       <c r="M118" s="3"/>
     </row>
-    <row r="119" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
@@ -8781,50 +8783,57 @@
       <c r="L119" s="3"/>
       <c r="M119" s="3"/>
     </row>
-    <row r="120" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B122" s="9"/>
     </row>
-    <row r="123" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B123" s="9"/>
     </row>
-    <row r="124" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B124" s="9"/>
     </row>
-    <row r="125" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B125" s="9"/>
     </row>
-    <row r="126" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B126" s="9"/>
     </row>
-    <row r="127" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B127" s="9"/>
     </row>
-    <row r="128" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B128" s="9"/>
     </row>
-    <row r="129" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B129" s="9"/>
     </row>
-    <row r="130" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B130" s="9"/>
     </row>
-    <row r="131" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B131" s="9"/>
     </row>
-    <row r="132" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B132" s="9"/>
     </row>
-    <row r="133" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B133" s="9"/>
     </row>
-    <row r="134" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B134" s="9"/>
     </row>
-    <row r="135" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J116:W116"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B78:B97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="B98:B106"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H116:I116"/>
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="J112:W112"/>
     <mergeCell ref="B14:B63"/>
@@ -8833,13 +8842,6 @@
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B111:G111"/>
-    <mergeCell ref="J116:W116"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B78:B97"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="B98:B106"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H116:I116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8853,7 +8855,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8865,7 +8867,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Link ya saca la espada al atacar (HAY QUE HACER QUE EL PROYECTIL SEA LA ESPADA NO LA FLECHA)
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
@@ -1313,6 +1313,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1322,6 +1325,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1346,9 +1379,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1357,36 +1387,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1475,19 +1475,19 @@
                   <c:v>16.160999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.160999999999998</c:v>
+                  <c:v>14.660999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.160999999999998</c:v>
+                  <c:v>14.660999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.160999999999998</c:v>
+                  <c:v>14.660999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.160999999999998</c:v>
+                  <c:v>14.660999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.160999999999998</c:v>
+                  <c:v>14.660999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,11 +1508,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-349567968"/>
-        <c:axId val="-349567424"/>
+        <c:axId val="1228711376"/>
+        <c:axId val="1228710288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-349567968"/>
+        <c:axId val="1228711376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1522,7 +1522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-349567424"/>
+        <c:crossAx val="1228710288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1530,7 +1530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-349567424"/>
+        <c:axId val="1228710288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1541,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-349567968"/>
+        <c:crossAx val="1228711376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1583,7 +1583,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1894,7 +1894,7 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R104" sqref="R104"/>
+      <selection activeCell="T104" sqref="T103:W104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1923,22 +1923,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="101" t="s">
+      <c r="J2" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="102"/>
-      <c r="T2" s="102"/>
-      <c r="U2" s="102"/>
-      <c r="V2" s="102"/>
-      <c r="W2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="104"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="89" t="s">
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="120" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="56" t="s">
@@ -2076,8 +2076,8 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="110"/>
-      <c r="C5" s="112" t="s">
+      <c r="B5" s="121"/>
+      <c r="C5" s="105" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="77" t="s">
@@ -2143,8 +2143,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="110"/>
-      <c r="C6" s="113"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="123"/>
       <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
@@ -2208,7 +2208,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="110"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2273,7 +2273,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="110"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="76" t="s">
         <v>16</v>
       </c>
@@ -2338,7 +2338,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="111"/>
+      <c r="B9" s="122"/>
       <c r="C9" s="36" t="s">
         <v>109</v>
       </c>
@@ -2403,7 +2403,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="118" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="93" t="s">
@@ -2458,7 +2458,7 @@
       <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2511,8 +2511,8 @@
       <c r="W11" s="28"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B12" s="107"/>
-      <c r="C12" s="112" t="s">
+      <c r="B12" s="118"/>
+      <c r="C12" s="105" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="49" t="s">
@@ -2566,8 +2566,8 @@
       <c r="W12" s="30"/>
     </row>
     <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="108"/>
-      <c r="C13" s="116"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="106"/>
       <c r="D13" s="37" t="s">
         <v>117</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="W13" s="41"/>
     </row>
     <row r="14" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="115" t="s">
         <v>119</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -2686,7 +2686,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="104"/>
+      <c r="B15" s="115"/>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2751,7 +2751,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="104"/>
+      <c r="B16" s="115"/>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
@@ -2816,7 +2816,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="104"/>
+      <c r="B17" s="115"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
@@ -2881,7 +2881,7 @@
       </c>
     </row>
     <row r="18" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="104"/>
+      <c r="B18" s="115"/>
       <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2946,7 +2946,7 @@
       </c>
     </row>
     <row r="19" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="104"/>
+      <c r="B19" s="115"/>
       <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
@@ -3011,7 +3011,7 @@
       </c>
     </row>
     <row r="20" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="104"/>
+      <c r="B20" s="115"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="21" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="104"/>
+      <c r="B21" s="115"/>
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
@@ -3141,7 +3141,7 @@
       </c>
     </row>
     <row r="22" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="104"/>
+      <c r="B22" s="115"/>
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
@@ -3206,7 +3206,7 @@
       </c>
     </row>
     <row r="23" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="104"/>
+      <c r="B23" s="115"/>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -3271,7 +3271,7 @@
       </c>
     </row>
     <row r="24" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="104"/>
+      <c r="B24" s="115"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
@@ -3336,7 +3336,7 @@
       </c>
     </row>
     <row r="25" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="104"/>
+      <c r="B25" s="115"/>
       <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3401,7 +3401,7 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="104"/>
+      <c r="B26" s="115"/>
       <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3466,7 +3466,7 @@
       </c>
     </row>
     <row r="27" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="104"/>
+      <c r="B27" s="115"/>
       <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
@@ -3531,7 +3531,7 @@
       </c>
     </row>
     <row r="28" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="104"/>
+      <c r="B28" s="115"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="29" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="104"/>
+      <c r="B29" s="115"/>
       <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
@@ -3661,7 +3661,7 @@
       </c>
     </row>
     <row r="30" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="104"/>
+      <c r="B30" s="115"/>
       <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
@@ -3726,7 +3726,7 @@
       </c>
     </row>
     <row r="31" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="104"/>
+      <c r="B31" s="115"/>
       <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
@@ -3791,7 +3791,7 @@
       </c>
     </row>
     <row r="32" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="104"/>
+      <c r="B32" s="115"/>
       <c r="C32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3856,7 +3856,7 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="104"/>
+      <c r="B33" s="115"/>
       <c r="C33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3921,7 +3921,7 @@
       </c>
     </row>
     <row r="34" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="104"/>
+      <c r="B34" s="115"/>
       <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3986,7 +3986,7 @@
       </c>
     </row>
     <row r="35" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="104"/>
+      <c r="B35" s="115"/>
       <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
@@ -4051,7 +4051,7 @@
       </c>
     </row>
     <row r="36" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="104"/>
+      <c r="B36" s="115"/>
       <c r="C36" s="4" t="s">
         <v>48</v>
       </c>
@@ -4116,7 +4116,7 @@
       </c>
     </row>
     <row r="37" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="104"/>
+      <c r="B37" s="115"/>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
@@ -4181,7 +4181,7 @@
       </c>
     </row>
     <row r="38" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="104"/>
+      <c r="B38" s="115"/>
       <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
     </row>
     <row r="39" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="104"/>
+      <c r="B39" s="115"/>
       <c r="C39" s="4" t="s">
         <v>51</v>
       </c>
@@ -4311,7 +4311,7 @@
       </c>
     </row>
     <row r="40" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="104"/>
+      <c r="B40" s="115"/>
       <c r="C40" s="4" t="s">
         <v>52</v>
       </c>
@@ -4376,7 +4376,7 @@
       </c>
     </row>
     <row r="41" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="104"/>
+      <c r="B41" s="115"/>
       <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4441,7 +4441,7 @@
       </c>
     </row>
     <row r="42" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="104"/>
+      <c r="B42" s="115"/>
       <c r="C42" s="4" t="s">
         <v>54</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="104"/>
+      <c r="B43" s="115"/>
       <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
@@ -4571,7 +4571,7 @@
       </c>
     </row>
     <row r="44" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="104"/>
+      <c r="B44" s="115"/>
       <c r="C44" s="4" t="s">
         <v>56</v>
       </c>
@@ -4636,7 +4636,7 @@
       </c>
     </row>
     <row r="45" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="104"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="4" t="s">
         <v>57</v>
       </c>
@@ -4701,7 +4701,7 @@
       </c>
     </row>
     <row r="46" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="104"/>
+      <c r="B46" s="115"/>
       <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
@@ -4766,7 +4766,7 @@
       </c>
     </row>
     <row r="47" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="104"/>
+      <c r="B47" s="115"/>
       <c r="C47" s="4" t="s">
         <v>59</v>
       </c>
@@ -4831,7 +4831,7 @@
       </c>
     </row>
     <row r="48" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="104"/>
+      <c r="B48" s="115"/>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
@@ -4896,7 +4896,7 @@
       </c>
     </row>
     <row r="49" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="104"/>
+      <c r="B49" s="115"/>
       <c r="C49" s="18" t="s">
         <v>61</v>
       </c>
@@ -4961,7 +4961,7 @@
       </c>
     </row>
     <row r="50" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="104"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="18" t="s">
         <v>77</v>
       </c>
@@ -5014,7 +5014,7 @@
       <c r="W50" s="28"/>
     </row>
     <row r="51" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="104"/>
+      <c r="B51" s="115"/>
       <c r="C51" s="18" t="s">
         <v>78</v>
       </c>
@@ -5067,7 +5067,7 @@
       <c r="W51" s="28"/>
     </row>
     <row r="52" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="104"/>
+      <c r="B52" s="115"/>
       <c r="C52" s="18" t="s">
         <v>79</v>
       </c>
@@ -5120,7 +5120,7 @@
       <c r="W52" s="28"/>
     </row>
     <row r="53" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="104"/>
+      <c r="B53" s="115"/>
       <c r="C53" s="18" t="s">
         <v>80</v>
       </c>
@@ -5173,7 +5173,7 @@
       <c r="W53" s="28"/>
     </row>
     <row r="54" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="104"/>
+      <c r="B54" s="115"/>
       <c r="C54" s="18" t="s">
         <v>81</v>
       </c>
@@ -5226,7 +5226,7 @@
       <c r="W54" s="28"/>
     </row>
     <row r="55" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="104"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="18" t="s">
         <v>82</v>
       </c>
@@ -5279,7 +5279,7 @@
       <c r="W55" s="28"/>
     </row>
     <row r="56" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="104"/>
+      <c r="B56" s="115"/>
       <c r="C56" s="18" t="s">
         <v>83</v>
       </c>
@@ -5332,7 +5332,7 @@
       <c r="W56" s="28"/>
     </row>
     <row r="57" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="104"/>
+      <c r="B57" s="115"/>
       <c r="C57" s="18" t="s">
         <v>84</v>
       </c>
@@ -5385,7 +5385,7 @@
       <c r="W57" s="28"/>
     </row>
     <row r="58" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="104"/>
+      <c r="B58" s="115"/>
       <c r="C58" s="18" t="s">
         <v>85</v>
       </c>
@@ -5438,7 +5438,7 @@
       <c r="W58" s="28"/>
     </row>
     <row r="59" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="104"/>
+      <c r="B59" s="115"/>
       <c r="C59" s="18" t="s">
         <v>86</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="W59" s="28"/>
     </row>
     <row r="60" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="104"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="18" t="s">
         <v>87</v>
       </c>
@@ -5544,7 +5544,7 @@
       <c r="W60" s="28"/>
     </row>
     <row r="61" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="104"/>
+      <c r="B61" s="115"/>
       <c r="C61" s="18" t="s">
         <v>88</v>
       </c>
@@ -5597,7 +5597,7 @@
       <c r="W61" s="28"/>
     </row>
     <row r="62" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="104"/>
+      <c r="B62" s="115"/>
       <c r="C62" s="18" t="s">
         <v>89</v>
       </c>
@@ -5650,7 +5650,7 @@
       <c r="W62" s="28"/>
     </row>
     <row r="63" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="105"/>
+      <c r="B63" s="116"/>
       <c r="C63" s="36" t="s">
         <v>90</v>
       </c>
@@ -5703,7 +5703,7 @@
       <c r="W63" s="41"/>
     </row>
     <row r="64" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="106" t="s">
+      <c r="B64" s="117" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="32" t="s">
@@ -5770,7 +5770,7 @@
       </c>
     </row>
     <row r="65" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="104"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="18" t="s">
         <v>64</v>
       </c>
@@ -5825,7 +5825,7 @@
       <c r="W65" s="28"/>
     </row>
     <row r="66" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="104"/>
+      <c r="B66" s="115"/>
       <c r="C66" s="18" t="s">
         <v>65</v>
       </c>
@@ -5878,7 +5878,7 @@
       <c r="W66" s="28"/>
     </row>
     <row r="67" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="104"/>
+      <c r="B67" s="115"/>
       <c r="C67" s="18" t="s">
         <v>66</v>
       </c>
@@ -5931,7 +5931,7 @@
       <c r="W67" s="28"/>
     </row>
     <row r="68" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="104"/>
+      <c r="B68" s="115"/>
       <c r="C68" s="18" t="s">
         <v>67</v>
       </c>
@@ -5984,7 +5984,7 @@
       <c r="W68" s="28"/>
     </row>
     <row r="69" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="104"/>
+      <c r="B69" s="115"/>
       <c r="C69" s="18" t="s">
         <v>68</v>
       </c>
@@ -6037,7 +6037,7 @@
       <c r="W69" s="28"/>
     </row>
     <row r="70" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="104"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="18" t="s">
         <v>69</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="W70" s="28"/>
     </row>
     <row r="71" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="104"/>
+      <c r="B71" s="115"/>
       <c r="C71" s="18" t="s">
         <v>70</v>
       </c>
@@ -6143,7 +6143,7 @@
       <c r="W71" s="28"/>
     </row>
     <row r="72" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="104"/>
+      <c r="B72" s="115"/>
       <c r="C72" s="18" t="s">
         <v>71</v>
       </c>
@@ -6196,7 +6196,7 @@
       <c r="W72" s="28"/>
     </row>
     <row r="73" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="104"/>
+      <c r="B73" s="115"/>
       <c r="C73" s="18" t="s">
         <v>72</v>
       </c>
@@ -6249,7 +6249,7 @@
       <c r="W73" s="28"/>
     </row>
     <row r="74" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="104"/>
+      <c r="B74" s="115"/>
       <c r="C74" s="18" t="s">
         <v>73</v>
       </c>
@@ -6302,7 +6302,7 @@
       <c r="W74" s="28"/>
     </row>
     <row r="75" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="104"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="18" t="s">
         <v>74</v>
       </c>
@@ -6355,7 +6355,7 @@
       <c r="W75" s="28"/>
     </row>
     <row r="76" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="104"/>
+      <c r="B76" s="115"/>
       <c r="C76" s="18" t="s">
         <v>75</v>
       </c>
@@ -6408,7 +6408,7 @@
       <c r="W76" s="28"/>
     </row>
     <row r="77" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="105"/>
+      <c r="B77" s="116"/>
       <c r="C77" s="36" t="s">
         <v>76</v>
       </c>
@@ -6461,7 +6461,7 @@
       <c r="W77" s="41"/>
     </row>
     <row r="78" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="117" t="s">
+      <c r="B78" s="107" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="6" t="s">
@@ -6528,7 +6528,7 @@
       </c>
     </row>
     <row r="79" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="118"/>
+      <c r="B79" s="108"/>
       <c r="C79" s="4" t="s">
         <v>26</v>
       </c>
@@ -6593,7 +6593,7 @@
       </c>
     </row>
     <row r="80" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="118"/>
+      <c r="B80" s="108"/>
       <c r="C80" s="4" t="s">
         <v>28</v>
       </c>
@@ -6658,7 +6658,7 @@
       </c>
     </row>
     <row r="81" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="118"/>
+      <c r="B81" s="108"/>
       <c r="C81" s="4" t="s">
         <v>29</v>
       </c>
@@ -6723,7 +6723,7 @@
       </c>
     </row>
     <row r="82" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="118"/>
+      <c r="B82" s="108"/>
       <c r="C82" s="4" t="s">
         <v>30</v>
       </c>
@@ -6788,7 +6788,7 @@
       </c>
     </row>
     <row r="83" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="118"/>
+      <c r="B83" s="108"/>
       <c r="C83" s="4" t="s">
         <v>31</v>
       </c>
@@ -6853,7 +6853,7 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="118"/>
+      <c r="B84" s="108"/>
       <c r="C84" s="4" t="s">
         <v>32</v>
       </c>
@@ -6918,7 +6918,7 @@
       </c>
     </row>
     <row r="85" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="118"/>
+      <c r="B85" s="108"/>
       <c r="C85" s="4" t="s">
         <v>33</v>
       </c>
@@ -6983,7 +6983,7 @@
       </c>
     </row>
     <row r="86" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="118"/>
+      <c r="B86" s="108"/>
       <c r="C86" s="4" t="s">
         <v>34</v>
       </c>
@@ -7048,7 +7048,7 @@
       </c>
     </row>
     <row r="87" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="118"/>
+      <c r="B87" s="108"/>
       <c r="C87" s="4" t="s">
         <v>35</v>
       </c>
@@ -7113,7 +7113,7 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="118"/>
+      <c r="B88" s="108"/>
       <c r="C88" s="4" t="s">
         <v>36</v>
       </c>
@@ -7178,7 +7178,7 @@
       </c>
     </row>
     <row r="89" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="118"/>
+      <c r="B89" s="108"/>
       <c r="C89" s="4" t="s">
         <v>37</v>
       </c>
@@ -7243,7 +7243,7 @@
       </c>
     </row>
     <row r="90" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="118"/>
+      <c r="B90" s="108"/>
       <c r="C90" s="4" t="s">
         <v>38</v>
       </c>
@@ -7308,7 +7308,7 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="118"/>
+      <c r="B91" s="108"/>
       <c r="C91" s="4" t="s">
         <v>39</v>
       </c>
@@ -7373,7 +7373,7 @@
       </c>
     </row>
     <row r="92" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="118"/>
+      <c r="B92" s="108"/>
       <c r="C92" s="4" t="s">
         <v>40</v>
       </c>
@@ -7438,7 +7438,7 @@
       </c>
     </row>
     <row r="93" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="118"/>
+      <c r="B93" s="108"/>
       <c r="C93" s="4" t="s">
         <v>41</v>
       </c>
@@ -7503,7 +7503,7 @@
       </c>
     </row>
     <row r="94" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="118"/>
+      <c r="B94" s="108"/>
       <c r="C94" s="4" t="s">
         <v>120</v>
       </c>
@@ -7568,7 +7568,7 @@
       </c>
     </row>
     <row r="95" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="118"/>
+      <c r="B95" s="108"/>
       <c r="C95" s="4" t="s">
         <v>121</v>
       </c>
@@ -7633,7 +7633,7 @@
       </c>
     </row>
     <row r="96" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="118"/>
+      <c r="B96" s="108"/>
       <c r="C96" s="4" t="s">
         <v>42</v>
       </c>
@@ -7698,7 +7698,7 @@
       </c>
     </row>
     <row r="97" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="119"/>
+      <c r="B97" s="109"/>
       <c r="C97" s="36" t="s">
         <v>92</v>
       </c>
@@ -7751,10 +7751,10 @@
       <c r="W97" s="41"/>
     </row>
     <row r="98" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="122" t="s">
+      <c r="B98" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="C98" s="120" t="s">
+      <c r="C98" s="110" t="s">
         <v>94</v>
       </c>
       <c r="D98" s="6" t="s">
@@ -7820,8 +7820,8 @@
       </c>
     </row>
     <row r="99" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="122"/>
-      <c r="C99" s="121"/>
+      <c r="B99" s="112"/>
+      <c r="C99" s="111"/>
       <c r="D99" s="4" t="s">
         <v>96</v>
       </c>
@@ -7885,8 +7885,8 @@
       </c>
     </row>
     <row r="100" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="122"/>
-      <c r="C100" s="121"/>
+      <c r="B100" s="112"/>
+      <c r="C100" s="111"/>
       <c r="D100" s="4" t="s">
         <v>97</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
     </row>
     <row r="101" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="122"/>
+      <c r="B101" s="112"/>
       <c r="C101" s="18" t="s">
         <v>115</v>
       </c>
@@ -8003,7 +8003,7 @@
       <c r="W101" s="99"/>
     </row>
     <row r="102" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="122"/>
+      <c r="B102" s="112"/>
       <c r="C102" s="18" t="s">
         <v>98</v>
       </c>
@@ -8056,7 +8056,7 @@
       <c r="W102" s="99"/>
     </row>
     <row r="103" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="122"/>
+      <c r="B103" s="112"/>
       <c r="C103" s="18" t="s">
         <v>99</v>
       </c>
@@ -8075,43 +8075,53 @@
       </c>
       <c r="I103" s="31">
         <f t="shared" si="1"/>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="J103" s="50">
+        <v>0</v>
+      </c>
+      <c r="K103" s="50">
+        <v>0</v>
+      </c>
+      <c r="L103" s="50">
+        <v>0</v>
+      </c>
+      <c r="M103" s="50">
+        <v>0</v>
+      </c>
+      <c r="N103" s="50">
+        <v>0</v>
+      </c>
+      <c r="O103" s="50">
+        <v>0</v>
+      </c>
+      <c r="P103" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="50">
+        <v>0</v>
+      </c>
+      <c r="R103" s="101">
         <v>0.76</v>
       </c>
-      <c r="J103" s="50">
-        <v>0</v>
-      </c>
-      <c r="K103" s="50">
-        <v>0</v>
-      </c>
-      <c r="L103" s="50">
-        <v>0</v>
-      </c>
-      <c r="M103" s="50">
-        <v>0</v>
-      </c>
-      <c r="N103" s="50">
-        <v>0</v>
-      </c>
-      <c r="O103" s="50">
-        <v>0</v>
-      </c>
-      <c r="P103" s="50">
-        <v>0</v>
-      </c>
-      <c r="Q103" s="50">
-        <v>0</v>
-      </c>
-      <c r="R103" s="125">
-        <v>0.76</v>
-      </c>
-      <c r="S103" s="98"/>
-      <c r="T103" s="98"/>
-      <c r="U103" s="98"/>
-      <c r="V103" s="98"/>
-      <c r="W103" s="99"/>
+      <c r="S103" s="67">
+        <v>1.5</v>
+      </c>
+      <c r="T103" s="67">
+        <v>0</v>
+      </c>
+      <c r="U103" s="67">
+        <v>0</v>
+      </c>
+      <c r="V103" s="67">
+        <v>0</v>
+      </c>
+      <c r="W103" s="67">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="122"/>
+      <c r="B104" s="112"/>
       <c r="C104" s="18" t="s">
         <v>100</v>
       </c>
@@ -8176,7 +8186,7 @@
       </c>
     </row>
     <row r="105" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="122"/>
+      <c r="B105" s="112"/>
       <c r="C105" s="18" t="s">
         <v>101</v>
       </c>
@@ -8229,7 +8239,7 @@
       <c r="W105" s="99"/>
     </row>
     <row r="106" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="123"/>
+      <c r="B106" s="113"/>
       <c r="C106" s="18" t="s">
         <v>102</v>
       </c>
@@ -8516,21 +8526,21 @@
       </c>
     </row>
     <row r="111" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="114" t="s">
+      <c r="B111" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="C111" s="115"/>
-      <c r="D111" s="115"/>
-      <c r="E111" s="115"/>
-      <c r="F111" s="115"/>
-      <c r="G111" s="115"/>
+      <c r="C111" s="125"/>
+      <c r="D111" s="125"/>
+      <c r="E111" s="125"/>
+      <c r="F111" s="125"/>
+      <c r="G111" s="125"/>
       <c r="H111" s="27">
         <f t="shared" ref="H111:W111" si="2">SUM(H4:H110)</f>
         <v>35.800000000000004</v>
       </c>
       <c r="I111" s="14">
         <f t="shared" si="2"/>
-        <v>19.638999999999999</v>
+        <v>21.138999999999999</v>
       </c>
       <c r="J111" s="12">
         <f t="shared" si="2"/>
@@ -8570,7 +8580,7 @@
       </c>
       <c r="S111" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="T111" s="15">
         <f t="shared" si="2"/>
@@ -8598,22 +8608,22 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
-      <c r="J112" s="101" t="s">
+      <c r="J112" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="K112" s="102"/>
-      <c r="L112" s="102"/>
-      <c r="M112" s="102"/>
-      <c r="N112" s="102"/>
-      <c r="O112" s="102"/>
-      <c r="P112" s="102"/>
-      <c r="Q112" s="102"/>
-      <c r="R112" s="102"/>
-      <c r="S112" s="102"/>
-      <c r="T112" s="102"/>
-      <c r="U112" s="102"/>
-      <c r="V112" s="102"/>
-      <c r="W112" s="103"/>
+      <c r="K112" s="103"/>
+      <c r="L112" s="103"/>
+      <c r="M112" s="103"/>
+      <c r="N112" s="103"/>
+      <c r="O112" s="103"/>
+      <c r="P112" s="103"/>
+      <c r="Q112" s="103"/>
+      <c r="R112" s="103"/>
+      <c r="S112" s="103"/>
+      <c r="T112" s="103"/>
+      <c r="U112" s="103"/>
+      <c r="V112" s="103"/>
+      <c r="W112" s="104"/>
     </row>
     <row r="113" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="2"/>
@@ -8638,10 +8648,10 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="101" t="s">
+      <c r="H114" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="I114" s="124"/>
+      <c r="I114" s="114"/>
       <c r="J114" s="13">
         <f>H111-J111</f>
         <v>35.800000000000004</v>
@@ -8680,23 +8690,23 @@
       </c>
       <c r="S114" s="13">
         <f t="shared" si="3"/>
-        <v>16.160999999999998</v>
+        <v>14.660999999999998</v>
       </c>
       <c r="T114" s="13">
         <f t="shared" si="3"/>
-        <v>16.160999999999998</v>
+        <v>14.660999999999998</v>
       </c>
       <c r="U114" s="13">
         <f t="shared" si="3"/>
-        <v>16.160999999999998</v>
+        <v>14.660999999999998</v>
       </c>
       <c r="V114" s="13">
         <f t="shared" si="3"/>
-        <v>16.160999999999998</v>
+        <v>14.660999999999998</v>
       </c>
       <c r="W114" s="13">
         <f t="shared" si="3"/>
-        <v>16.160999999999998</v>
+        <v>14.660999999999998</v>
       </c>
     </row>
     <row r="115" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8719,27 +8729,27 @@
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="H116" s="101" t="s">
+      <c r="H116" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="I116" s="102"/>
-      <c r="J116" s="101">
+      <c r="I116" s="103"/>
+      <c r="J116" s="102">
         <f>H111-I111</f>
-        <v>16.161000000000005</v>
-      </c>
-      <c r="K116" s="102"/>
-      <c r="L116" s="102"/>
-      <c r="M116" s="102"/>
-      <c r="N116" s="102"/>
-      <c r="O116" s="102"/>
-      <c r="P116" s="102"/>
-      <c r="Q116" s="102"/>
-      <c r="R116" s="102"/>
-      <c r="S116" s="102"/>
-      <c r="T116" s="102"/>
-      <c r="U116" s="102"/>
-      <c r="V116" s="102"/>
-      <c r="W116" s="103"/>
+        <v>14.661000000000005</v>
+      </c>
+      <c r="K116" s="103"/>
+      <c r="L116" s="103"/>
+      <c r="M116" s="103"/>
+      <c r="N116" s="103"/>
+      <c r="O116" s="103"/>
+      <c r="P116" s="103"/>
+      <c r="Q116" s="103"/>
+      <c r="R116" s="103"/>
+      <c r="S116" s="103"/>
+      <c r="T116" s="103"/>
+      <c r="U116" s="103"/>
+      <c r="V116" s="103"/>
+      <c r="W116" s="104"/>
     </row>
     <row r="117" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B117" s="3"/>
@@ -8827,13 +8837,6 @@
     <row r="135" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="J116:W116"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B78:B97"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="B98:B106"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H116:I116"/>
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="J112:W112"/>
     <mergeCell ref="B14:B63"/>
@@ -8842,6 +8845,13 @@
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B111:G111"/>
+    <mergeCell ref="J116:W116"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B78:B97"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="B98:B106"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H116:I116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Por fin puesto dungeon (el json) en el juego. alomejor se complica programar las salas
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 2 SampleTextStudio.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acanut\Documents\ENTI\MAP\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\MAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1034,7 +1034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1304,6 +1304,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1313,6 +1315,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1337,9 +1369,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1349,35 +1378,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1398,7 +1404,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1465,19 +1471,19 @@
                   <c:v>14.910999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.420999999999998</c:v>
+                  <c:v>8.070999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.420999999999998</c:v>
+                  <c:v>8.070999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.420999999999998</c:v>
+                  <c:v>8.070999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.420999999999998</c:v>
+                  <c:v>8.070999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.420999999999998</c:v>
+                  <c:v>8.070999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1538,7 +1544,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1595,7 +1600,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1670,6 +1675,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1705,6 +1727,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1883,11 +1922,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X65" sqref="X65"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U89" sqref="U89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
@@ -1913,22 +1952,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="103" t="s">
+      <c r="J2" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="105"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="89" t="s">
@@ -1999,7 +2038,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="123" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="56" t="s">
@@ -2066,8 +2105,8 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="112"/>
-      <c r="C5" s="114" t="s">
+      <c r="B5" s="124"/>
+      <c r="C5" s="108" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="77" t="s">
@@ -2133,8 +2172,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="112"/>
-      <c r="C6" s="115"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="126"/>
       <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
@@ -2198,7 +2237,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="112"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2263,7 +2302,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="112"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="76" t="s">
         <v>16</v>
       </c>
@@ -2328,7 +2367,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="113"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="36" t="s">
         <v>104</v>
       </c>
@@ -2393,7 +2432,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="121" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="93" t="s">
@@ -2448,7 +2487,7 @@
       <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="109"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2501,8 +2540,8 @@
       <c r="W11" s="28"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="109"/>
-      <c r="C12" s="114" t="s">
+      <c r="B12" s="121"/>
+      <c r="C12" s="108" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="49" t="s">
@@ -2556,8 +2595,8 @@
       <c r="W12" s="30"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="110"/>
-      <c r="C13" s="118"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="109"/>
       <c r="D13" s="37" t="s">
         <v>112</v>
       </c>
@@ -2609,7 +2648,7 @@
       <c r="W13" s="41"/>
     </row>
     <row r="14" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="118" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -2676,7 +2715,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="106"/>
+      <c r="B15" s="118"/>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2741,7 +2780,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="106"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
@@ -2806,7 +2845,7 @@
       </c>
     </row>
     <row r="17" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="106"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
@@ -2871,7 +2910,7 @@
       </c>
     </row>
     <row r="18" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="106"/>
+      <c r="B18" s="118"/>
       <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2936,7 +2975,7 @@
       </c>
     </row>
     <row r="19" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="106"/>
+      <c r="B19" s="118"/>
       <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
@@ -3001,7 +3040,7 @@
       </c>
     </row>
     <row r="20" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="106"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3066,7 +3105,7 @@
       </c>
     </row>
     <row r="21" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="106"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
@@ -3131,7 +3170,7 @@
       </c>
     </row>
     <row r="22" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="106"/>
+      <c r="B22" s="118"/>
       <c r="C22" s="4" t="s">
         <v>34</v>
       </c>
@@ -3196,7 +3235,7 @@
       </c>
     </row>
     <row r="23" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="106"/>
+      <c r="B23" s="118"/>
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -3261,7 +3300,7 @@
       </c>
     </row>
     <row r="24" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="106"/>
+      <c r="B24" s="118"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
@@ -3326,7 +3365,7 @@
       </c>
     </row>
     <row r="25" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="106"/>
+      <c r="B25" s="118"/>
       <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3391,7 +3430,7 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="106"/>
+      <c r="B26" s="118"/>
       <c r="C26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3456,7 +3495,7 @@
       </c>
     </row>
     <row r="27" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="106"/>
+      <c r="B27" s="118"/>
       <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
@@ -3521,7 +3560,7 @@
       </c>
     </row>
     <row r="28" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="106"/>
+      <c r="B28" s="118"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
@@ -3586,7 +3625,7 @@
       </c>
     </row>
     <row r="29" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="106"/>
+      <c r="B29" s="118"/>
       <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
@@ -3651,7 +3690,7 @@
       </c>
     </row>
     <row r="30" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="106"/>
+      <c r="B30" s="118"/>
       <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
@@ -3716,7 +3755,7 @@
       </c>
     </row>
     <row r="31" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="106"/>
+      <c r="B31" s="118"/>
       <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
@@ -3781,7 +3820,7 @@
       </c>
     </row>
     <row r="32" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="106"/>
+      <c r="B32" s="118"/>
       <c r="C32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3846,7 +3885,7 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="106"/>
+      <c r="B33" s="118"/>
       <c r="C33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3911,7 +3950,7 @@
       </c>
     </row>
     <row r="34" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="106"/>
+      <c r="B34" s="118"/>
       <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3976,7 +4015,7 @@
       </c>
     </row>
     <row r="35" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="106"/>
+      <c r="B35" s="118"/>
       <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
@@ -4041,7 +4080,7 @@
       </c>
     </row>
     <row r="36" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="106"/>
+      <c r="B36" s="118"/>
       <c r="C36" s="4" t="s">
         <v>48</v>
       </c>
@@ -4106,7 +4145,7 @@
       </c>
     </row>
     <row r="37" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="106"/>
+      <c r="B37" s="118"/>
       <c r="C37" s="4" t="s">
         <v>49</v>
       </c>
@@ -4171,7 +4210,7 @@
       </c>
     </row>
     <row r="38" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="106"/>
+      <c r="B38" s="118"/>
       <c r="C38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4236,7 +4275,7 @@
       </c>
     </row>
     <row r="39" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="106"/>
+      <c r="B39" s="118"/>
       <c r="C39" s="4" t="s">
         <v>51</v>
       </c>
@@ -4301,7 +4340,7 @@
       </c>
     </row>
     <row r="40" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="106"/>
+      <c r="B40" s="118"/>
       <c r="C40" s="4" t="s">
         <v>52</v>
       </c>
@@ -4366,7 +4405,7 @@
       </c>
     </row>
     <row r="41" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="106"/>
+      <c r="B41" s="118"/>
       <c r="C41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4431,7 +4470,7 @@
       </c>
     </row>
     <row r="42" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="106"/>
+      <c r="B42" s="118"/>
       <c r="C42" s="4" t="s">
         <v>54</v>
       </c>
@@ -4496,7 +4535,7 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="106"/>
+      <c r="B43" s="118"/>
       <c r="C43" s="4" t="s">
         <v>55</v>
       </c>
@@ -4561,7 +4600,7 @@
       </c>
     </row>
     <row r="44" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="106"/>
+      <c r="B44" s="118"/>
       <c r="C44" s="4" t="s">
         <v>56</v>
       </c>
@@ -4626,7 +4665,7 @@
       </c>
     </row>
     <row r="45" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="106"/>
+      <c r="B45" s="118"/>
       <c r="C45" s="4" t="s">
         <v>57</v>
       </c>
@@ -4691,7 +4730,7 @@
       </c>
     </row>
     <row r="46" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="106"/>
+      <c r="B46" s="118"/>
       <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
@@ -4756,7 +4795,7 @@
       </c>
     </row>
     <row r="47" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="106"/>
+      <c r="B47" s="118"/>
       <c r="C47" s="4" t="s">
         <v>59</v>
       </c>
@@ -4821,7 +4860,7 @@
       </c>
     </row>
     <row r="48" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="106"/>
+      <c r="B48" s="118"/>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
@@ -4886,7 +4925,7 @@
       </c>
     </row>
     <row r="49" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="106"/>
+      <c r="B49" s="118"/>
       <c r="C49" s="18" t="s">
         <v>61</v>
       </c>
@@ -4951,7 +4990,7 @@
       </c>
     </row>
     <row r="50" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="106"/>
+      <c r="B50" s="118"/>
       <c r="C50" s="18" t="s">
         <v>72</v>
       </c>
@@ -5004,7 +5043,7 @@
       <c r="W50" s="28"/>
     </row>
     <row r="51" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="106"/>
+      <c r="B51" s="118"/>
       <c r="C51" s="18" t="s">
         <v>73</v>
       </c>
@@ -5057,7 +5096,7 @@
       <c r="W51" s="28"/>
     </row>
     <row r="52" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="106"/>
+      <c r="B52" s="118"/>
       <c r="C52" s="18" t="s">
         <v>74</v>
       </c>
@@ -5110,7 +5149,7 @@
       <c r="W52" s="28"/>
     </row>
     <row r="53" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="106"/>
+      <c r="B53" s="118"/>
       <c r="C53" s="18" t="s">
         <v>75</v>
       </c>
@@ -5163,7 +5202,7 @@
       <c r="W53" s="28"/>
     </row>
     <row r="54" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="106"/>
+      <c r="B54" s="118"/>
       <c r="C54" s="18" t="s">
         <v>76</v>
       </c>
@@ -5216,7 +5255,7 @@
       <c r="W54" s="28"/>
     </row>
     <row r="55" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="106"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="18" t="s">
         <v>77</v>
       </c>
@@ -5269,7 +5308,7 @@
       <c r="W55" s="28"/>
     </row>
     <row r="56" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="106"/>
+      <c r="B56" s="118"/>
       <c r="C56" s="18" t="s">
         <v>78</v>
       </c>
@@ -5322,7 +5361,7 @@
       <c r="W56" s="28"/>
     </row>
     <row r="57" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="106"/>
+      <c r="B57" s="118"/>
       <c r="C57" s="18" t="s">
         <v>79</v>
       </c>
@@ -5375,7 +5414,7 @@
       <c r="W57" s="28"/>
     </row>
     <row r="58" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="106"/>
+      <c r="B58" s="118"/>
       <c r="C58" s="18" t="s">
         <v>80</v>
       </c>
@@ -5428,7 +5467,7 @@
       <c r="W58" s="28"/>
     </row>
     <row r="59" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="106"/>
+      <c r="B59" s="118"/>
       <c r="C59" s="18" t="s">
         <v>81</v>
       </c>
@@ -5481,7 +5520,7 @@
       <c r="W59" s="28"/>
     </row>
     <row r="60" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="106"/>
+      <c r="B60" s="118"/>
       <c r="C60" s="18" t="s">
         <v>82</v>
       </c>
@@ -5534,7 +5573,7 @@
       <c r="W60" s="28"/>
     </row>
     <row r="61" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="106"/>
+      <c r="B61" s="118"/>
       <c r="C61" s="18" t="s">
         <v>83</v>
       </c>
@@ -5587,7 +5626,7 @@
       <c r="W61" s="28"/>
     </row>
     <row r="62" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="106"/>
+      <c r="B62" s="118"/>
       <c r="C62" s="18" t="s">
         <v>84</v>
       </c>
@@ -5640,7 +5679,7 @@
       <c r="W62" s="28"/>
     </row>
     <row r="63" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="107"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="36" t="s">
         <v>85</v>
       </c>
@@ -5693,7 +5732,7 @@
       <c r="W63" s="41"/>
     </row>
     <row r="64" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="108" t="s">
+      <c r="B64" s="120" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="32" t="s">
@@ -5760,7 +5799,7 @@
       </c>
     </row>
     <row r="65" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="106"/>
+      <c r="B65" s="118"/>
       <c r="C65" s="18" t="s">
         <v>64</v>
       </c>
@@ -5825,7 +5864,7 @@
       </c>
     </row>
     <row r="66" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="106"/>
+      <c r="B66" s="118"/>
       <c r="C66" s="18" t="s">
         <v>65</v>
       </c>
@@ -5890,7 +5929,7 @@
       </c>
     </row>
     <row r="67" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="106"/>
+      <c r="B67" s="118"/>
       <c r="C67" s="18" t="s">
         <v>66</v>
       </c>
@@ -5955,7 +5994,7 @@
       </c>
     </row>
     <row r="68" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="106"/>
+      <c r="B68" s="118"/>
       <c r="C68" s="18" t="s">
         <v>67</v>
       </c>
@@ -6020,7 +6059,7 @@
       </c>
     </row>
     <row r="69" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="106"/>
+      <c r="B69" s="118"/>
       <c r="C69" s="18" t="s">
         <v>68</v>
       </c>
@@ -6085,7 +6124,7 @@
       </c>
     </row>
     <row r="70" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="106"/>
+      <c r="B70" s="118"/>
       <c r="C70" s="18" t="s">
         <v>69</v>
       </c>
@@ -6150,7 +6189,7 @@
       </c>
     </row>
     <row r="71" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="106"/>
+      <c r="B71" s="118"/>
       <c r="C71" s="18" t="s">
         <v>70</v>
       </c>
@@ -6215,7 +6254,7 @@
       </c>
     </row>
     <row r="72" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="106"/>
+      <c r="B72" s="118"/>
       <c r="C72" s="36" t="s">
         <v>71</v>
       </c>
@@ -6263,7 +6302,7 @@
       <c r="R72" s="96">
         <v>0</v>
       </c>
-      <c r="S72" s="127">
+      <c r="S72" s="103">
         <v>0.1</v>
       </c>
       <c r="T72" s="70">
@@ -6280,7 +6319,7 @@
       </c>
     </row>
     <row r="73" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="119" t="s">
+      <c r="B73" s="110" t="s">
         <v>86</v>
       </c>
       <c r="C73" s="6" t="s">
@@ -6347,7 +6386,7 @@
       </c>
     </row>
     <row r="74" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="120"/>
+      <c r="B74" s="111"/>
       <c r="C74" s="4" t="s">
         <v>26</v>
       </c>
@@ -6412,7 +6451,7 @@
       </c>
     </row>
     <row r="75" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="120"/>
+      <c r="B75" s="111"/>
       <c r="C75" s="4" t="s">
         <v>28</v>
       </c>
@@ -6477,7 +6516,7 @@
       </c>
     </row>
     <row r="76" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="120"/>
+      <c r="B76" s="111"/>
       <c r="C76" s="4" t="s">
         <v>29</v>
       </c>
@@ -6542,7 +6581,7 @@
       </c>
     </row>
     <row r="77" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="120"/>
+      <c r="B77" s="111"/>
       <c r="C77" s="4" t="s">
         <v>30</v>
       </c>
@@ -6607,7 +6646,7 @@
       </c>
     </row>
     <row r="78" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="120"/>
+      <c r="B78" s="111"/>
       <c r="C78" s="4" t="s">
         <v>31</v>
       </c>
@@ -6672,7 +6711,7 @@
       </c>
     </row>
     <row r="79" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="120"/>
+      <c r="B79" s="111"/>
       <c r="C79" s="4" t="s">
         <v>32</v>
       </c>
@@ -6737,7 +6776,7 @@
       </c>
     </row>
     <row r="80" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="120"/>
+      <c r="B80" s="111"/>
       <c r="C80" s="4" t="s">
         <v>33</v>
       </c>
@@ -6802,7 +6841,7 @@
       </c>
     </row>
     <row r="81" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="120"/>
+      <c r="B81" s="111"/>
       <c r="C81" s="4" t="s">
         <v>34</v>
       </c>
@@ -6867,7 +6906,7 @@
       </c>
     </row>
     <row r="82" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="120"/>
+      <c r="B82" s="111"/>
       <c r="C82" s="4" t="s">
         <v>35</v>
       </c>
@@ -6932,7 +6971,7 @@
       </c>
     </row>
     <row r="83" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="120"/>
+      <c r="B83" s="111"/>
       <c r="C83" s="4" t="s">
         <v>36</v>
       </c>
@@ -6997,7 +7036,7 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="120"/>
+      <c r="B84" s="111"/>
       <c r="C84" s="4" t="s">
         <v>37</v>
       </c>
@@ -7062,7 +7101,7 @@
       </c>
     </row>
     <row r="85" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="120"/>
+      <c r="B85" s="111"/>
       <c r="C85" s="4" t="s">
         <v>38</v>
       </c>
@@ -7127,7 +7166,7 @@
       </c>
     </row>
     <row r="86" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="120"/>
+      <c r="B86" s="111"/>
       <c r="C86" s="4" t="s">
         <v>39</v>
       </c>
@@ -7192,7 +7231,7 @@
       </c>
     </row>
     <row r="87" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="120"/>
+      <c r="B87" s="111"/>
       <c r="C87" s="4" t="s">
         <v>40</v>
       </c>
@@ -7257,7 +7296,7 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="120"/>
+      <c r="B88" s="111"/>
       <c r="C88" s="4" t="s">
         <v>41</v>
       </c>
@@ -7322,7 +7361,7 @@
       </c>
     </row>
     <row r="89" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="120"/>
+      <c r="B89" s="111"/>
       <c r="C89" s="4" t="s">
         <v>115</v>
       </c>
@@ -7387,7 +7426,7 @@
       </c>
     </row>
     <row r="90" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="120"/>
+      <c r="B90" s="111"/>
       <c r="C90" s="4" t="s">
         <v>116</v>
       </c>
@@ -7452,7 +7491,7 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="120"/>
+      <c r="B91" s="111"/>
       <c r="C91" s="4" t="s">
         <v>42</v>
       </c>
@@ -7517,7 +7556,7 @@
       </c>
     </row>
     <row r="92" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="121"/>
+      <c r="B92" s="112"/>
       <c r="C92" s="36" t="s">
         <v>87</v>
       </c>
@@ -7536,7 +7575,7 @@
       </c>
       <c r="I92" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.35</v>
       </c>
       <c r="J92" s="51">
         <v>0</v>
@@ -7562,20 +7601,30 @@
       <c r="Q92" s="51">
         <v>0</v>
       </c>
-      <c r="R92" s="128">
-        <v>0</v>
-      </c>
-      <c r="S92" s="40"/>
-      <c r="T92" s="40"/>
-      <c r="U92" s="40"/>
-      <c r="V92" s="40"/>
-      <c r="W92" s="41"/>
+      <c r="R92" s="104">
+        <v>0</v>
+      </c>
+      <c r="S92" s="129">
+        <v>2.35</v>
+      </c>
+      <c r="T92" s="129">
+        <v>0</v>
+      </c>
+      <c r="U92" s="129">
+        <v>0</v>
+      </c>
+      <c r="V92" s="129">
+        <v>0</v>
+      </c>
+      <c r="W92" s="130">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="124" t="s">
+      <c r="B93" s="115" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="122" t="s">
+      <c r="C93" s="113" t="s">
         <v>89</v>
       </c>
       <c r="D93" s="6" t="s">
@@ -7641,8 +7690,8 @@
       </c>
     </row>
     <row r="94" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="124"/>
-      <c r="C94" s="123"/>
+      <c r="B94" s="115"/>
+      <c r="C94" s="114"/>
       <c r="D94" s="4" t="s">
         <v>91</v>
       </c>
@@ -7706,8 +7755,8 @@
       </c>
     </row>
     <row r="95" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="124"/>
-      <c r="C95" s="123"/>
+      <c r="B95" s="115"/>
+      <c r="C95" s="114"/>
       <c r="D95" s="4" t="s">
         <v>92</v>
       </c>
@@ -7771,7 +7820,7 @@
       </c>
     </row>
     <row r="96" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="124"/>
+      <c r="B96" s="115"/>
       <c r="C96" s="18" t="s">
         <v>110</v>
       </c>
@@ -7824,7 +7873,7 @@
       <c r="W96" s="99"/>
     </row>
     <row r="97" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="124"/>
+      <c r="B97" s="115"/>
       <c r="C97" s="18" t="s">
         <v>93</v>
       </c>
@@ -7877,7 +7926,7 @@
       <c r="W97" s="99"/>
     </row>
     <row r="98" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="124"/>
+      <c r="B98" s="115"/>
       <c r="C98" s="18" t="s">
         <v>94</v>
       </c>
@@ -7942,7 +7991,7 @@
       </c>
     </row>
     <row r="99" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="124"/>
+      <c r="B99" s="115"/>
       <c r="C99" s="18" t="s">
         <v>95</v>
       </c>
@@ -8007,7 +8056,7 @@
       </c>
     </row>
     <row r="100" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="124"/>
+      <c r="B100" s="115"/>
       <c r="C100" s="18" t="s">
         <v>96</v>
       </c>
@@ -8060,7 +8109,7 @@
       <c r="W100" s="99"/>
     </row>
     <row r="101" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="125"/>
+      <c r="B101" s="116"/>
       <c r="C101" s="18" t="s">
         <v>97</v>
       </c>
@@ -8347,76 +8396,76 @@
       </c>
     </row>
     <row r="106" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="116" t="s">
+      <c r="B106" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="C106" s="117"/>
-      <c r="D106" s="117"/>
-      <c r="E106" s="117"/>
-      <c r="F106" s="117"/>
-      <c r="G106" s="117"/>
+      <c r="C106" s="128"/>
+      <c r="D106" s="128"/>
+      <c r="E106" s="128"/>
+      <c r="F106" s="128"/>
+      <c r="G106" s="128"/>
       <c r="H106" s="27">
-        <f>SUM(H4:H105)</f>
+        <f t="shared" ref="H106:W106" si="2">SUM(H4:H105)</f>
         <v>34.550000000000004</v>
       </c>
       <c r="I106" s="14">
-        <f>SUM(I4:I105)</f>
-        <v>24.128999999999994</v>
+        <f t="shared" si="2"/>
+        <v>26.478999999999996</v>
       </c>
       <c r="J106" s="12">
-        <f>SUM(J4:J105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K106" s="13">
-        <f>SUM(K4:K105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L106" s="13">
-        <f>SUM(L4:L105)</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="M106" s="15">
-        <f>SUM(M4:M105)</f>
+        <f t="shared" si="2"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N106" s="15">
-        <f>SUM(N4:N105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O106" s="15">
-        <f>SUM(O4:O105)</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="P106" s="15">
-        <f>SUM(P4:P105)</f>
+        <f t="shared" si="2"/>
         <v>8.9750000000000014</v>
       </c>
       <c r="Q106" s="15">
-        <f>SUM(Q4:Q105)</f>
+        <f t="shared" si="2"/>
         <v>3.4870000000000001</v>
       </c>
       <c r="R106" s="15">
-        <f>SUM(R4:R105)</f>
+        <f t="shared" si="2"/>
         <v>4.407</v>
       </c>
       <c r="S106" s="15">
-        <f>SUM(S4:S105)</f>
-        <v>4.49</v>
+        <f t="shared" si="2"/>
+        <v>6.84</v>
       </c>
       <c r="T106" s="15">
-        <f>SUM(T4:T105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U106" s="15">
-        <f>SUM(U4:U105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V106" s="15">
-        <f>SUM(V4:V105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W106" s="15">
-        <f>SUM(W4:W105)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -8429,22 +8478,22 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
-      <c r="J107" s="103" t="s">
+      <c r="J107" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="K107" s="104"/>
-      <c r="L107" s="104"/>
-      <c r="M107" s="104"/>
-      <c r="N107" s="104"/>
-      <c r="O107" s="104"/>
-      <c r="P107" s="104"/>
-      <c r="Q107" s="104"/>
-      <c r="R107" s="104"/>
-      <c r="S107" s="104"/>
-      <c r="T107" s="104"/>
-      <c r="U107" s="104"/>
-      <c r="V107" s="104"/>
-      <c r="W107" s="105"/>
+      <c r="K107" s="106"/>
+      <c r="L107" s="106"/>
+      <c r="M107" s="106"/>
+      <c r="N107" s="106"/>
+      <c r="O107" s="106"/>
+      <c r="P107" s="106"/>
+      <c r="Q107" s="106"/>
+      <c r="R107" s="106"/>
+      <c r="S107" s="106"/>
+      <c r="T107" s="106"/>
+      <c r="U107" s="106"/>
+      <c r="V107" s="106"/>
+      <c r="W107" s="107"/>
     </row>
     <row r="108" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="2"/>
@@ -8469,10 +8518,10 @@
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
-      <c r="H109" s="103" t="s">
+      <c r="H109" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="I109" s="126"/>
+      <c r="I109" s="117"/>
       <c r="J109" s="13">
         <f>H106-J106</f>
         <v>34.550000000000004</v>
@@ -8490,44 +8539,44 @@
         <v>34.28</v>
       </c>
       <c r="N109" s="13">
-        <f t="shared" ref="N109:W109" si="2">M109-N106</f>
+        <f t="shared" ref="N109:W109" si="3">M109-N106</f>
         <v>34.28</v>
       </c>
       <c r="O109" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.78</v>
       </c>
       <c r="P109" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22.805</v>
       </c>
       <c r="Q109" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19.317999999999998</v>
       </c>
       <c r="R109" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.910999999999998</v>
       </c>
       <c r="S109" s="13">
-        <f t="shared" si="2"/>
-        <v>10.420999999999998</v>
+        <f t="shared" si="3"/>
+        <v>8.070999999999998</v>
       </c>
       <c r="T109" s="13">
-        <f t="shared" si="2"/>
-        <v>10.420999999999998</v>
+        <f t="shared" si="3"/>
+        <v>8.070999999999998</v>
       </c>
       <c r="U109" s="13">
-        <f t="shared" si="2"/>
-        <v>10.420999999999998</v>
+        <f t="shared" si="3"/>
+        <v>8.070999999999998</v>
       </c>
       <c r="V109" s="13">
-        <f t="shared" si="2"/>
-        <v>10.420999999999998</v>
+        <f t="shared" si="3"/>
+        <v>8.070999999999998</v>
       </c>
       <c r="W109" s="13">
-        <f t="shared" si="2"/>
-        <v>10.420999999999998</v>
+        <f t="shared" si="3"/>
+        <v>8.070999999999998</v>
       </c>
     </row>
     <row r="110" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8550,27 +8599,27 @@
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
-      <c r="H111" s="103" t="s">
+      <c r="H111" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="I111" s="104"/>
-      <c r="J111" s="103">
+      <c r="I111" s="106"/>
+      <c r="J111" s="105">
         <f>H106-I106</f>
-        <v>10.42100000000001</v>
-      </c>
-      <c r="K111" s="104"/>
-      <c r="L111" s="104"/>
-      <c r="M111" s="104"/>
-      <c r="N111" s="104"/>
-      <c r="O111" s="104"/>
-      <c r="P111" s="104"/>
-      <c r="Q111" s="104"/>
-      <c r="R111" s="104"/>
-      <c r="S111" s="104"/>
-      <c r="T111" s="104"/>
-      <c r="U111" s="104"/>
-      <c r="V111" s="104"/>
-      <c r="W111" s="105"/>
+        <v>8.0710000000000086</v>
+      </c>
+      <c r="K111" s="106"/>
+      <c r="L111" s="106"/>
+      <c r="M111" s="106"/>
+      <c r="N111" s="106"/>
+      <c r="O111" s="106"/>
+      <c r="P111" s="106"/>
+      <c r="Q111" s="106"/>
+      <c r="R111" s="106"/>
+      <c r="S111" s="106"/>
+      <c r="T111" s="106"/>
+      <c r="U111" s="106"/>
+      <c r="V111" s="106"/>
+      <c r="W111" s="107"/>
     </row>
     <row r="112" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B112" s="3"/>
@@ -8658,13 +8707,6 @@
     <row r="130" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="J111:W111"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B73:B92"/>
-    <mergeCell ref="C93:C95"/>
-    <mergeCell ref="B93:B101"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="H111:I111"/>
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="J107:W107"/>
     <mergeCell ref="B14:B63"/>
@@ -8673,6 +8715,13 @@
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B106:G106"/>
+    <mergeCell ref="J111:W111"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B73:B92"/>
+    <mergeCell ref="C93:C95"/>
+    <mergeCell ref="B93:B101"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="H111:I111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8686,7 +8735,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8698,7 +8747,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>